<commit_message>
load diccionary ok, with error management
</commit_message>
<xml_diff>
--- a/src/common/bd/DiccionarioMultiX.xlsx
+++ b/src/common/bd/DiccionarioMultiX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Huerta\Documents\nhuerta\Proyectos\zeroco\BackEnd\src\common\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E434F3A-E25D-4F5B-9904-E0B6884D4182}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9A6E39D7-3659-46A1-AE58-514B3A64586A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D6A7E3F4-D4FA-4332-B22C-F7F93CCAE935}"/>
+    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6A7E3F4-D4FA-4332-B22C-F7F93CCAE935}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="140">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="656" uniqueCount="139">
   <si>
     <t>Gasolina</t>
   </si>
@@ -273,9 +273,6 @@
   </si>
   <si>
     <t>Fuentes móviles</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Medio terrestres </t>
   </si>
   <si>
     <t>Gas licuado de petróleo</t>
@@ -463,7 +460,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
-    <numFmt numFmtId="169" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
+    <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -558,14 +555,14 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="169" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="169" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="41" fontId="0" fillId="5" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -575,9 +572,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -925,10 +919,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAD24B2-CCAB-4B33-A88E-76925CA353A4}">
-  <dimension ref="A1:M69"/>
+  <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3:XFD3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -939,17 +933,17 @@
     <col min="4" max="4" width="10.08984375" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="8.6328125" style="3" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="14.90625" style="3" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="10.90625" style="3"/>
-    <col min="8" max="8" width="14.90625" style="3" customWidth="1"/>
-    <col min="9" max="9" width="10.90625" style="3"/>
-    <col min="10" max="10" width="34.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="27.54296875" style="3" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="44.6328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18.36328125" style="5" bestFit="1" customWidth="1"/>
-    <col min="14" max="16384" width="10.90625" style="3"/>
+    <col min="7" max="8" width="10.90625" style="3"/>
+    <col min="9" max="9" width="14.90625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="10.90625" style="3"/>
+    <col min="11" max="11" width="34.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="27.54296875" style="3" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="44.6328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="18.36328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="15" max="16384" width="10.90625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>69</v>
       </c>
@@ -969,26 +963,27 @@
         <v>74</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>131</v>
-      </c>
-      <c r="H1" s="2"/>
-      <c r="I1" s="1" t="s">
+        <v>130</v>
+      </c>
+      <c r="H1" s="1"/>
+      <c r="I1" s="2"/>
+      <c r="J1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="K1" s="1" t="s">
         <v>127</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="M1" s="10" t="s">
         <v>129</v>
       </c>
-      <c r="L1" s="11" t="s">
-        <v>130</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>133</v>
-      </c>
-    </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N1" s="1" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>1</v>
       </c>
@@ -1007,27 +1002,28 @@
       <c r="F2" s="5">
         <v>23210</v>
       </c>
-      <c r="G2" s="6" t="s">
-        <v>132</v>
+      <c r="G2" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H2" s="5"/>
-      <c r="I2" s="5" t="s">
+      <c r="I2" s="5"/>
+      <c r="J2" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J2" s="5" t="s">
+      <c r="K2" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K2" s="5" t="s">
+      <c r="L2" s="5" t="s">
         <v>77</v>
       </c>
-      <c r="L2" s="12" t="s">
+      <c r="M2" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M2" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N2" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A3" s="5">
         <v>1</v>
       </c>
@@ -1046,27 +1042,28 @@
       <c r="F3" s="5">
         <v>3580</v>
       </c>
-      <c r="G3" s="6" t="s">
-        <v>132</v>
+      <c r="G3" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H3" s="5"/>
-      <c r="I3" s="5" t="s">
+      <c r="I3" s="5"/>
+      <c r="J3" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="5" t="s">
+      <c r="K3" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K3" s="5" t="s">
-        <v>79</v>
-      </c>
-      <c r="L3" s="12" t="s">
+      <c r="L3" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="M3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="M3" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N3" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A4" s="5">
         <v>1</v>
       </c>
@@ -1085,27 +1082,28 @@
       <c r="F4" s="5">
         <v>1129243</v>
       </c>
-      <c r="G4" s="6" t="s">
-        <v>132</v>
+      <c r="G4" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H4" s="5"/>
-      <c r="I4" s="5" t="s">
+      <c r="I4" s="5"/>
+      <c r="J4" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J4" s="5" t="s">
+      <c r="K4" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K4" s="5" t="s">
+      <c r="L4" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L4" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M4" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M4" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N4" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A5" s="5">
         <v>1</v>
       </c>
@@ -1124,27 +1122,28 @@
       <c r="F5" s="5">
         <v>8951</v>
       </c>
-      <c r="G5" s="6" t="s">
-        <v>132</v>
+      <c r="G5" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H5" s="5"/>
-      <c r="I5" s="5" t="s">
+      <c r="I5" s="5"/>
+      <c r="J5" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J5" s="5" t="s">
+      <c r="K5" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K5" s="5" t="s">
+      <c r="L5" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L5" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M5" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M5" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N5" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A6" s="5">
         <v>1</v>
       </c>
@@ -1163,27 +1162,28 @@
       <c r="F6" s="5">
         <v>105022</v>
       </c>
-      <c r="G6" s="6" t="s">
-        <v>132</v>
+      <c r="G6" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H6" s="5"/>
-      <c r="I6" s="5" t="s">
+      <c r="I6" s="5"/>
+      <c r="J6" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J6" s="5" t="s">
+      <c r="K6" s="5" t="s">
         <v>76</v>
       </c>
-      <c r="K6" s="5" t="s">
+      <c r="L6" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="L6" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M6" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M6" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N6" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A7" s="5">
         <v>1</v>
       </c>
@@ -1202,27 +1202,28 @@
       <c r="F7" s="5">
         <v>21920</v>
       </c>
-      <c r="G7" s="6" t="s">
-        <v>132</v>
+      <c r="G7" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H7" s="5"/>
-      <c r="I7" s="5" t="s">
+      <c r="I7" s="5"/>
+      <c r="J7" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="5" t="s">
+      <c r="K7" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K7" s="5" t="s">
+      <c r="L7" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M7" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="L7" s="12" t="s">
-        <v>82</v>
-      </c>
-      <c r="M7" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N7" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A8" s="5">
         <v>1</v>
       </c>
@@ -1241,27 +1242,28 @@
       <c r="F8" s="5">
         <v>135132</v>
       </c>
-      <c r="G8" s="6" t="s">
-        <v>132</v>
+      <c r="G8" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H8" s="5"/>
-      <c r="I8" s="5" t="s">
+      <c r="I8" s="5"/>
+      <c r="J8" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J8" s="5" t="s">
+      <c r="K8" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L8" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K8" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L8" s="12" t="s">
-        <v>80</v>
-      </c>
-      <c r="M8" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M8" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="N8" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A9" s="5">
         <v>1</v>
       </c>
@@ -1280,27 +1282,28 @@
       <c r="F9" s="5">
         <v>700</v>
       </c>
-      <c r="G9" s="6" t="s">
-        <v>132</v>
+      <c r="G9" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H9" s="5"/>
-      <c r="I9" s="5" t="s">
+      <c r="I9" s="5"/>
+      <c r="J9" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J9" s="5" t="s">
+      <c r="K9" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L9" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K9" s="5" t="s">
+      <c r="M9" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="L9" s="12" t="s">
-        <v>85</v>
-      </c>
-      <c r="M9" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N9" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A10" s="5">
         <v>1</v>
       </c>
@@ -1319,27 +1322,28 @@
       <c r="F10" s="5">
         <v>5221203</v>
       </c>
-      <c r="G10" s="6" t="s">
-        <v>132</v>
+      <c r="G10" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H10" s="5"/>
-      <c r="I10" s="5" t="s">
+      <c r="I10" s="5"/>
+      <c r="J10" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="5" t="s">
+      <c r="K10" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K10" s="5" t="s">
-        <v>81</v>
-      </c>
-      <c r="L10" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="M10" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L10" s="5" t="s">
+        <v>80</v>
+      </c>
+      <c r="M10" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N10" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A11" s="5">
         <v>1</v>
       </c>
@@ -1358,27 +1362,28 @@
       <c r="F11" s="5">
         <v>756989</v>
       </c>
-      <c r="G11" s="6" t="s">
-        <v>132</v>
+      <c r="G11" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H11" s="5"/>
-      <c r="I11" s="5" t="s">
+      <c r="I11" s="5"/>
+      <c r="J11" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J11" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="K11" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L11" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L11" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="M11" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M11" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N11" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A12" s="5">
         <v>1</v>
       </c>
@@ -1397,27 +1402,28 @@
       <c r="F12" s="5">
         <v>3664514</v>
       </c>
-      <c r="G12" s="6" t="s">
-        <v>132</v>
+      <c r="G12" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H12" s="5"/>
-      <c r="I12" s="5" t="s">
+      <c r="I12" s="5"/>
+      <c r="J12" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J12" s="5" t="s">
-        <v>83</v>
-      </c>
       <c r="K12" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L12" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="L12" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="M12" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M12" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N12" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A13" s="5">
         <v>1</v>
       </c>
@@ -1436,27 +1442,28 @@
       <c r="F13" s="5">
         <v>35600</v>
       </c>
-      <c r="G13" s="6" t="s">
-        <v>132</v>
+      <c r="G13" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H13" s="5"/>
-      <c r="I13" s="5" t="s">
+      <c r="I13" s="5"/>
+      <c r="J13" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J13" s="5" t="s">
+      <c r="K13" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L13" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K13" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L13" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="M13" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M13" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N13" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A14" s="5">
         <v>1</v>
       </c>
@@ -1475,27 +1482,28 @@
       <c r="F14" s="5">
         <v>240434</v>
       </c>
-      <c r="G14" s="6" t="s">
-        <v>132</v>
+      <c r="G14" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H14" s="5"/>
-      <c r="I14" s="5" t="s">
+      <c r="I14" s="5"/>
+      <c r="J14" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="5" t="s">
+      <c r="K14" s="5" t="s">
         <v>78</v>
       </c>
-      <c r="K14" s="5" t="s">
-        <v>88</v>
-      </c>
-      <c r="L14" s="12" t="s">
-        <v>86</v>
-      </c>
-      <c r="M14" s="5" t="s">
-        <v>134</v>
-      </c>
-    </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="L14" s="5" t="s">
+        <v>87</v>
+      </c>
+      <c r="M14" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="N14" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A15" s="5">
         <v>1</v>
       </c>
@@ -1514,62 +1522,64 @@
       <c r="F15" s="5">
         <v>1191116</v>
       </c>
-      <c r="G15" s="6" t="s">
-        <v>132</v>
+      <c r="G15" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H15" s="5"/>
-      <c r="I15" s="5" t="s">
+      <c r="I15" s="5"/>
+      <c r="J15" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J15" s="5" t="s">
+      <c r="K15" s="5" t="s">
+        <v>82</v>
+      </c>
+      <c r="L15" s="5" t="s">
         <v>83</v>
       </c>
-      <c r="K15" s="5" t="s">
-        <v>84</v>
-      </c>
-      <c r="L15" s="12" t="s">
-        <v>87</v>
-      </c>
-      <c r="M15" s="5" t="s">
+      <c r="M15" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="N15" s="5" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="16" spans="1:14" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="6">
+        <v>1</v>
+      </c>
+      <c r="B16" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="6" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="6">
+        <v>15626</v>
+      </c>
+      <c r="G16" s="6" t="s">
+        <v>131</v>
+      </c>
+      <c r="H16" s="6"/>
+      <c r="I16" s="6"/>
+      <c r="J16" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="K16" s="6" t="s">
+        <v>88</v>
+      </c>
+      <c r="L16" s="6"/>
+      <c r="M16" s="12"/>
+      <c r="N16" s="6" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="16" spans="1:13" s="4" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="7">
-        <v>1</v>
-      </c>
-      <c r="B16" s="7" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="7">
-        <v>15626</v>
-      </c>
-      <c r="G16" s="7" t="s">
-        <v>132</v>
-      </c>
-      <c r="H16" s="7"/>
-      <c r="I16" s="7" t="s">
-        <v>75</v>
-      </c>
-      <c r="J16" s="7" t="s">
-        <v>89</v>
-      </c>
-      <c r="K16" s="7"/>
-      <c r="L16" s="13"/>
-      <c r="M16" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A17" s="5">
         <v>1</v>
       </c>
@@ -1588,27 +1598,28 @@
       <c r="F17" s="5">
         <v>709</v>
       </c>
-      <c r="G17" s="6" t="s">
-        <v>132</v>
+      <c r="G17" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H17" s="5"/>
-      <c r="I17" s="5" t="s">
+      <c r="I17" s="5"/>
+      <c r="J17" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J17" s="5" t="s">
+      <c r="K17" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L17" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="K17" s="5" t="s">
-        <v>90</v>
-      </c>
-      <c r="L17" s="12" t="s">
-        <v>90</v>
-      </c>
-      <c r="M17" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M17" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="N17" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="18" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A18" s="5">
         <v>1</v>
       </c>
@@ -1627,27 +1638,28 @@
       <c r="F18" s="5">
         <v>90</v>
       </c>
-      <c r="G18" s="6" t="s">
-        <v>132</v>
+      <c r="G18" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H18" s="5"/>
-      <c r="I18" s="5" t="s">
+      <c r="I18" s="5"/>
+      <c r="J18" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J18" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="K18" s="5" t="s">
-        <v>91</v>
-      </c>
-      <c r="L18" s="12" t="s">
-        <v>91</v>
-      </c>
-      <c r="M18" s="7" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.35">
+        <v>88</v>
+      </c>
+      <c r="L18" s="5" t="s">
+        <v>90</v>
+      </c>
+      <c r="M18" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="N18" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="19" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A19" s="5">
         <v>1</v>
       </c>
@@ -1666,438 +1678,450 @@
       <c r="F19" s="5">
         <v>136</v>
       </c>
-      <c r="G19" s="6" t="s">
-        <v>132</v>
+      <c r="G19" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H19" s="5"/>
-      <c r="I19" s="5" t="s">
+      <c r="I19" s="5"/>
+      <c r="J19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="J19" s="5" t="s">
-        <v>89</v>
-      </c>
       <c r="K19" s="5" t="s">
+        <v>88</v>
+      </c>
+      <c r="L19" s="5" t="s">
+        <v>91</v>
+      </c>
+      <c r="M19" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="N19" s="6" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="7">
+        <v>2</v>
+      </c>
+      <c r="B20" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="7">
+        <v>27914</v>
+      </c>
+      <c r="G20" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H20" s="7"/>
+      <c r="I20" s="7"/>
+      <c r="J20" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="L19" s="12" t="s">
+      <c r="K20" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L20" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="M20" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="N20" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="7">
+        <v>2</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="7">
+        <v>26738</v>
+      </c>
+      <c r="G21" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H21" s="7"/>
+      <c r="I21" s="7"/>
+      <c r="J21" s="7" t="s">
         <v>92</v>
       </c>
-      <c r="M19" s="7" t="s">
+      <c r="K21" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L21" s="7" t="s">
+        <v>96</v>
+      </c>
+      <c r="M21" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="N21" s="7" t="s">
         <v>135</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A20" s="8">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="7">
         <v>2</v>
       </c>
-      <c r="B20" s="8" t="s">
+      <c r="B22" s="7" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="8" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="8" t="s">
+      <c r="C22" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="7">
+        <v>4525740</v>
+      </c>
+      <c r="G22" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H22" s="7"/>
+      <c r="I22" s="7"/>
+      <c r="J22" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K22" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L22" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M22" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="N22" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="7">
+        <v>2</v>
+      </c>
+      <c r="B23" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="7">
+        <v>35683</v>
+      </c>
+      <c r="G23" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H23" s="7"/>
+      <c r="I23" s="7"/>
+      <c r="J23" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K23" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="L23" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M23" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="N23" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="7">
+        <v>2</v>
+      </c>
+      <c r="B24" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="7" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="8" t="s">
+      <c r="E24" s="7" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="8">
-        <v>27914</v>
-      </c>
-      <c r="G20" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H20" s="8"/>
-      <c r="I20" s="8" t="s">
+      <c r="F24" s="7">
+        <v>21344</v>
+      </c>
+      <c r="G24" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H24" s="7"/>
+      <c r="I24" s="7"/>
+      <c r="J24" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="K24" s="7" t="s">
         <v>93</v>
       </c>
-      <c r="J20" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K20" s="8" t="s">
-        <v>95</v>
-      </c>
-      <c r="L20" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="M20" s="8" t="s">
+      <c r="L24" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="M24" s="13" t="s">
+        <v>98</v>
+      </c>
+      <c r="N24" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="25" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A25" s="8">
+        <v>2</v>
+      </c>
+      <c r="B25" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="C25" s="8" t="s">
+        <v>28</v>
+      </c>
+      <c r="D25" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="E25" s="8" t="s">
+        <v>26</v>
+      </c>
+      <c r="F25" s="8">
+        <v>16327818</v>
+      </c>
+      <c r="G25" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="H25" s="8"/>
+      <c r="I25" s="8"/>
+      <c r="J25" s="8" t="s">
+        <v>92</v>
+      </c>
+      <c r="K25" s="8"/>
+      <c r="L25" s="8"/>
+      <c r="M25" s="14"/>
+      <c r="N25" s="7" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="26" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A26" s="7">
+        <v>3</v>
+      </c>
+      <c r="B26" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C26" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="D26" s="7" t="s">
+        <v>5</v>
+      </c>
+      <c r="E26" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F26" s="7">
+        <v>22773</v>
+      </c>
+      <c r="G26" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H26" s="7"/>
+      <c r="I26" s="7"/>
+      <c r="J26" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K26" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L26" s="7" t="s">
+        <v>101</v>
+      </c>
+      <c r="M26" s="13" t="s">
+        <v>102</v>
+      </c>
+      <c r="N26" s="7" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="7">
+        <v>3</v>
+      </c>
+      <c r="B27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="7" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="7">
+        <v>4203498</v>
+      </c>
+      <c r="G27" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H27" s="7"/>
+      <c r="I27" s="7"/>
+      <c r="J27" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K27" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L27" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M27" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="N27" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="7">
+        <v>3</v>
+      </c>
+      <c r="B28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C28" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="7" t="s">
+        <v>20</v>
+      </c>
+      <c r="F28" s="7">
+        <v>119043744</v>
+      </c>
+      <c r="G28" s="7" t="s">
+        <v>131</v>
+      </c>
+      <c r="H28" s="7"/>
+      <c r="I28" s="7"/>
+      <c r="J28" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="K28" s="7" t="s">
+        <v>100</v>
+      </c>
+      <c r="L28" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="M28" s="13" t="s">
+        <v>103</v>
+      </c>
+      <c r="N28" s="7" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="29" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A29" s="9">
+        <v>3</v>
+      </c>
+      <c r="B29" s="9" t="s">
+        <v>36</v>
+      </c>
+      <c r="C29" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="D29" s="9" t="s">
+        <v>9</v>
+      </c>
+      <c r="E29" s="9" t="s">
+        <v>38</v>
+      </c>
+      <c r="F29" s="9">
+        <v>2517</v>
+      </c>
+      <c r="G29" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H29" s="9"/>
+      <c r="I29" s="9"/>
+      <c r="J29" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K29" s="9"/>
+      <c r="L29" s="9"/>
+      <c r="M29" s="15"/>
+      <c r="N29" s="9" t="s">
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A21" s="8">
-        <v>2</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="8" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="8">
-        <v>26738</v>
-      </c>
-      <c r="G21" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H21" s="8"/>
-      <c r="I21" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J21" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K21" s="8" t="s">
-        <v>97</v>
-      </c>
-      <c r="L21" s="14" t="s">
-        <v>96</v>
-      </c>
-      <c r="M21" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A22" s="8">
-        <v>2</v>
-      </c>
-      <c r="B22" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="8" t="s">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A30" s="9">
+        <v>3</v>
+      </c>
+      <c r="B30" s="9" t="s">
+        <v>39</v>
+      </c>
+      <c r="C30" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E22" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="8">
-        <v>4525740</v>
-      </c>
-      <c r="G22" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H22" s="8"/>
-      <c r="I22" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J22" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K22" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L22" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="M22" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A23" s="8">
-        <v>2</v>
-      </c>
-      <c r="B23" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="8">
-        <v>35683</v>
-      </c>
-      <c r="G23" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H23" s="8"/>
-      <c r="I23" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J23" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K23" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L23" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="M23" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A24" s="8">
-        <v>2</v>
-      </c>
-      <c r="B24" s="8" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="8" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="8" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="8">
-        <v>21344</v>
-      </c>
-      <c r="G24" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H24" s="8"/>
-      <c r="I24" s="8" t="s">
-        <v>93</v>
-      </c>
-      <c r="J24" s="8" t="s">
-        <v>94</v>
-      </c>
-      <c r="K24" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="L24" s="14" t="s">
-        <v>99</v>
-      </c>
-      <c r="M24" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A25" s="9">
-        <v>2</v>
-      </c>
-      <c r="B25" s="9" t="s">
-        <v>29</v>
-      </c>
-      <c r="C25" s="9" t="s">
-        <v>28</v>
-      </c>
-      <c r="D25" s="9" t="s">
-        <v>9</v>
-      </c>
-      <c r="E25" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="F25" s="9">
-        <v>16327818</v>
-      </c>
-      <c r="G25" s="9" t="s">
-        <v>132</v>
-      </c>
-      <c r="H25" s="9"/>
-      <c r="I25" s="9" t="s">
-        <v>93</v>
-      </c>
-      <c r="J25" s="9"/>
-      <c r="K25" s="9"/>
-      <c r="L25" s="15"/>
-      <c r="M25" s="8" t="s">
-        <v>136</v>
-      </c>
-    </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A26" s="8">
-        <v>3</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C26" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="D26" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="E26" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F26" s="8">
-        <v>22773</v>
-      </c>
-      <c r="G26" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H26" s="8"/>
-      <c r="I26" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J26" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K26" s="8" t="s">
-        <v>102</v>
-      </c>
-      <c r="L26" s="14" t="s">
-        <v>103</v>
-      </c>
-      <c r="M26" s="8" t="s">
+      <c r="E30" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="F30" s="9">
+        <v>0</v>
+      </c>
+      <c r="G30" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H30" s="9"/>
+      <c r="I30" s="9"/>
+      <c r="J30" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K30" s="9"/>
+      <c r="L30" s="9"/>
+      <c r="M30" s="15"/>
+      <c r="N30" s="9" t="s">
         <v>134</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A27" s="8">
-        <v>3</v>
-      </c>
-      <c r="B27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C27" s="8" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="8" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="8">
-        <v>4203498</v>
-      </c>
-      <c r="G27" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H27" s="8"/>
-      <c r="I27" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J27" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K27" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="L27" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="M27" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A28" s="8">
-        <v>3</v>
-      </c>
-      <c r="B28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="8" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="8" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="8">
-        <v>119043744</v>
-      </c>
-      <c r="G28" s="8" t="s">
-        <v>132</v>
-      </c>
-      <c r="H28" s="8"/>
-      <c r="I28" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="J28" s="8" t="s">
-        <v>101</v>
-      </c>
-      <c r="K28" s="8" t="s">
-        <v>33</v>
-      </c>
-      <c r="L28" s="14" t="s">
-        <v>104</v>
-      </c>
-      <c r="M28" s="8" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A29" s="10">
-        <v>3</v>
-      </c>
-      <c r="B29" s="10" t="s">
-        <v>36</v>
-      </c>
-      <c r="C29" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="D29" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="E29" s="10" t="s">
-        <v>38</v>
-      </c>
-      <c r="F29" s="10">
-        <v>2517</v>
-      </c>
-      <c r="G29" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H29" s="10"/>
-      <c r="I29" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J29" s="10"/>
-      <c r="K29" s="10"/>
-      <c r="L29" s="16"/>
-      <c r="M29" s="10" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A30" s="10">
-        <v>3</v>
-      </c>
-      <c r="B30" s="10" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>40</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>20</v>
-      </c>
-      <c r="F30" s="10">
-        <v>0</v>
-      </c>
-      <c r="G30" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H30" s="10"/>
-      <c r="I30" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J30" s="10"/>
-      <c r="K30" s="10"/>
-      <c r="L30" s="16"/>
-      <c r="M30" s="10" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A31" s="5">
         <v>3</v>
       </c>
@@ -2116,27 +2140,28 @@
       <c r="F31" s="5">
         <v>23308</v>
       </c>
-      <c r="G31" s="6" t="s">
-        <v>132</v>
+      <c r="G31" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H31" s="5"/>
-      <c r="I31" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I31" s="5"/>
       <c r="J31" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L31" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K31" s="5" t="s">
+      <c r="M31" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="L31" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="M31" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N31" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A32" s="5">
         <v>3</v>
       </c>
@@ -2155,27 +2180,28 @@
       <c r="F32" s="5">
         <v>212000</v>
       </c>
-      <c r="G32" s="6" t="s">
-        <v>132</v>
+      <c r="G32" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H32" s="5"/>
-      <c r="I32" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I32" s="5"/>
       <c r="J32" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K32" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L32" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K32" s="5" t="s">
+      <c r="M32" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="L32" s="12" t="s">
-        <v>107</v>
-      </c>
-      <c r="M32" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N32" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="33" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A33" s="5">
         <v>3</v>
       </c>
@@ -2194,60 +2220,62 @@
       <c r="F33" s="5">
         <v>5470</v>
       </c>
-      <c r="G33" s="6" t="s">
-        <v>132</v>
+      <c r="G33" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H33" s="5"/>
-      <c r="I33" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I33" s="5"/>
       <c r="J33" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L33" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K33" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L33" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="M33" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A34" s="10">
-        <v>3</v>
-      </c>
-      <c r="B34" s="10" t="s">
+      <c r="M33" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="N33" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="34" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A34" s="9">
+        <v>3</v>
+      </c>
+      <c r="B34" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C34" s="10" t="s">
+      <c r="C34" s="9" t="s">
         <v>42</v>
       </c>
-      <c r="D34" s="10" t="s">
+      <c r="D34" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="E34" s="10" t="s">
+      <c r="E34" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F34" s="10">
+      <c r="F34" s="9">
         <v>0</v>
       </c>
-      <c r="G34" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H34" s="10"/>
-      <c r="I34" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J34" s="10"/>
-      <c r="K34" s="10"/>
-      <c r="L34" s="16"/>
-      <c r="M34" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G34" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H34" s="9"/>
+      <c r="I34" s="9"/>
+      <c r="J34" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K34" s="9"/>
+      <c r="L34" s="9"/>
+      <c r="M34" s="15"/>
+      <c r="N34" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="35" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A35" s="5">
         <v>3</v>
       </c>
@@ -2266,27 +2294,28 @@
       <c r="F35" s="5">
         <v>32984</v>
       </c>
-      <c r="G35" s="6" t="s">
-        <v>132</v>
+      <c r="G35" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H35" s="5"/>
-      <c r="I35" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I35" s="5"/>
       <c r="J35" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L35" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K35" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L35" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="M35" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M35" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="N35" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="36" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A36" s="5">
         <v>3</v>
       </c>
@@ -2305,27 +2334,28 @@
       <c r="F36" s="5">
         <v>3100</v>
       </c>
-      <c r="G36" s="6" t="s">
-        <v>132</v>
+      <c r="G36" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H36" s="5"/>
-      <c r="I36" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I36" s="5"/>
       <c r="J36" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K36" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L36" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K36" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L36" s="12" t="s">
-        <v>109</v>
-      </c>
-      <c r="M36" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M36" s="11" t="s">
+        <v>108</v>
+      </c>
+      <c r="N36" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="37" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A37" s="5">
         <v>3</v>
       </c>
@@ -2344,27 +2374,28 @@
       <c r="F37" s="5">
         <v>5000</v>
       </c>
-      <c r="G37" s="6" t="s">
-        <v>132</v>
+      <c r="G37" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H37" s="5"/>
-      <c r="I37" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I37" s="5"/>
       <c r="J37" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K37" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L37" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K37" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L37" s="12" t="s">
-        <v>108</v>
-      </c>
-      <c r="M37" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M37" s="11" t="s">
+        <v>107</v>
+      </c>
+      <c r="N37" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A38" s="5">
         <v>3</v>
       </c>
@@ -2383,60 +2414,62 @@
       <c r="F38" s="5">
         <v>1871000</v>
       </c>
-      <c r="G38" s="6" t="s">
-        <v>132</v>
+      <c r="G38" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H38" s="5"/>
-      <c r="I38" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I38" s="5"/>
       <c r="J38" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K38" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L38" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M38" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="L38" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="M38" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A39" s="10">
-        <v>3</v>
-      </c>
-      <c r="B39" s="10" t="s">
+      <c r="N38" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="39" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A39" s="9">
+        <v>3</v>
+      </c>
+      <c r="B39" s="9" t="s">
         <v>39</v>
       </c>
-      <c r="C39" s="10" t="s">
+      <c r="C39" s="9" t="s">
         <v>45</v>
       </c>
-      <c r="D39" s="10" t="s">
+      <c r="D39" s="9" t="s">
         <v>2</v>
       </c>
-      <c r="E39" s="10" t="s">
+      <c r="E39" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="F39" s="10">
+      <c r="F39" s="9">
         <v>0</v>
       </c>
-      <c r="G39" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H39" s="10"/>
-      <c r="I39" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J39" s="10"/>
-      <c r="K39" s="10"/>
-      <c r="L39" s="16"/>
-      <c r="M39" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G39" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H39" s="9"/>
+      <c r="I39" s="9"/>
+      <c r="J39" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K39" s="9"/>
+      <c r="L39" s="9"/>
+      <c r="M39" s="15"/>
+      <c r="N39" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="40" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A40" s="5">
         <v>3</v>
       </c>
@@ -2455,27 +2488,28 @@
       <c r="F40" s="5">
         <v>1435000</v>
       </c>
-      <c r="G40" s="6" t="s">
-        <v>132</v>
+      <c r="G40" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H40" s="5"/>
-      <c r="I40" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I40" s="5"/>
       <c r="J40" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K40" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L40" s="5" t="s">
+        <v>109</v>
+      </c>
+      <c r="M40" s="11" t="s">
         <v>110</v>
       </c>
-      <c r="L40" s="12" t="s">
-        <v>111</v>
-      </c>
-      <c r="M40" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N40" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="41" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A41" s="5">
         <v>3</v>
       </c>
@@ -2494,27 +2528,28 @@
       <c r="F41" s="5">
         <v>38000</v>
       </c>
-      <c r="G41" s="6" t="s">
-        <v>132</v>
+      <c r="G41" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H41" s="5"/>
-      <c r="I41" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I41" s="5"/>
       <c r="J41" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K41" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L41" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M41" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L41" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M41" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N41" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="42" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A42" s="5">
         <v>3</v>
       </c>
@@ -2533,27 +2568,28 @@
       <c r="F42" s="5">
         <v>21599</v>
       </c>
-      <c r="G42" s="6" t="s">
-        <v>132</v>
+      <c r="G42" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H42" s="5"/>
-      <c r="I42" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I42" s="5"/>
       <c r="J42" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K42" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L42" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M42" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L42" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M42" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N42" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="43" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A43" s="5">
         <v>3</v>
       </c>
@@ -2572,27 +2608,28 @@
       <c r="F43" s="5">
         <v>46584</v>
       </c>
-      <c r="G43" s="6" t="s">
-        <v>132</v>
+      <c r="G43" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H43" s="5"/>
-      <c r="I43" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I43" s="5"/>
       <c r="J43" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K43" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L43" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K43" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L43" s="12" t="s">
+      <c r="M43" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="M43" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N43" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="44" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A44" s="5">
         <v>3</v>
       </c>
@@ -2611,27 +2648,28 @@
       <c r="F44" s="5">
         <v>697475</v>
       </c>
-      <c r="G44" s="6" t="s">
-        <v>132</v>
+      <c r="G44" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H44" s="5"/>
-      <c r="I44" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I44" s="5"/>
       <c r="J44" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K44" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L44" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K44" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L44" s="12" t="s">
+      <c r="M44" s="11" t="s">
         <v>47</v>
       </c>
-      <c r="M44" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N44" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="45" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A45" s="5">
         <v>3</v>
       </c>
@@ -2650,23 +2688,24 @@
       <c r="F45" s="5">
         <v>176231</v>
       </c>
-      <c r="G45" s="6" t="s">
-        <v>132</v>
+      <c r="G45" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H45" s="5"/>
-      <c r="I45" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I45" s="5"/>
       <c r="J45" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K45" s="5"/>
-      <c r="L45" s="12"/>
-      <c r="M45" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K45" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L45" s="5"/>
+      <c r="M45" s="11"/>
+      <c r="N45" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A46" s="5">
         <v>3</v>
       </c>
@@ -2685,23 +2724,24 @@
       <c r="F46" s="5">
         <v>7620</v>
       </c>
-      <c r="G46" s="6" t="s">
-        <v>132</v>
+      <c r="G46" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H46" s="5"/>
-      <c r="I46" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I46" s="5"/>
       <c r="J46" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K46" s="5"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K46" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L46" s="5"/>
+      <c r="M46" s="11"/>
+      <c r="N46" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A47" s="5">
         <v>3</v>
       </c>
@@ -2720,23 +2760,24 @@
       <c r="F47" s="5">
         <v>138</v>
       </c>
-      <c r="G47" s="6" t="s">
-        <v>132</v>
+      <c r="G47" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H47" s="5"/>
-      <c r="I47" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I47" s="5"/>
       <c r="J47" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K47" s="5"/>
-      <c r="L47" s="12"/>
-      <c r="M47" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L47" s="5"/>
+      <c r="M47" s="11"/>
+      <c r="N47" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A48" s="5">
         <v>3</v>
       </c>
@@ -2755,23 +2796,24 @@
       <c r="F48" s="5">
         <v>18482</v>
       </c>
-      <c r="G48" s="6" t="s">
-        <v>132</v>
+      <c r="G48" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H48" s="5"/>
-      <c r="I48" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I48" s="5"/>
       <c r="J48" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K48" s="5"/>
-      <c r="L48" s="12"/>
-      <c r="M48" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L48" s="5"/>
+      <c r="M48" s="11"/>
+      <c r="N48" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A49" s="5">
         <v>3</v>
       </c>
@@ -2790,23 +2832,24 @@
       <c r="F49" s="5">
         <v>493</v>
       </c>
-      <c r="G49" s="6" t="s">
-        <v>132</v>
+      <c r="G49" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H49" s="5"/>
-      <c r="I49" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I49" s="5"/>
       <c r="J49" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K49" s="5"/>
-      <c r="L49" s="12"/>
-      <c r="M49" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L49" s="5"/>
+      <c r="M49" s="11"/>
+      <c r="N49" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="50" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A50" s="5">
         <v>3</v>
       </c>
@@ -2825,27 +2868,28 @@
       <c r="F50" s="5">
         <v>10463</v>
       </c>
-      <c r="G50" s="6" t="s">
-        <v>132</v>
+      <c r="G50" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H50" s="5"/>
-      <c r="I50" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I50" s="5"/>
       <c r="J50" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L50" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K50" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L50" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="M50" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M50" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N50" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="51" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A51" s="5">
         <v>3</v>
       </c>
@@ -2864,27 +2908,28 @@
       <c r="F51" s="5">
         <v>408687</v>
       </c>
-      <c r="G51" s="6" t="s">
-        <v>132</v>
+      <c r="G51" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H51" s="5"/>
-      <c r="I51" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I51" s="5"/>
       <c r="J51" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L51" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K51" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L51" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="M51" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M51" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N51" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="52" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A52" s="5">
         <v>3</v>
       </c>
@@ -2903,27 +2948,28 @@
       <c r="F52" s="5">
         <v>164080</v>
       </c>
-      <c r="G52" s="6" t="s">
-        <v>132</v>
+      <c r="G52" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H52" s="5"/>
-      <c r="I52" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I52" s="5"/>
       <c r="J52" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K52" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L52" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="K52" s="5" t="s">
-        <v>106</v>
-      </c>
-      <c r="L52" s="12" t="s">
-        <v>114</v>
-      </c>
-      <c r="M52" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="M52" s="11" t="s">
+        <v>113</v>
+      </c>
+      <c r="N52" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="53" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A53" s="5">
         <v>3</v>
       </c>
@@ -2942,23 +2988,24 @@
       <c r="F53" s="5">
         <v>491610</v>
       </c>
-      <c r="G53" s="6" t="s">
-        <v>132</v>
+      <c r="G53" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H53" s="5"/>
-      <c r="I53" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I53" s="5"/>
       <c r="J53" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K53" s="5"/>
-      <c r="L53" s="12"/>
-      <c r="M53" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K53" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L53" s="5"/>
+      <c r="M53" s="11"/>
+      <c r="N53" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="54" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A54" s="5">
         <v>3</v>
       </c>
@@ -2977,23 +3024,24 @@
       <c r="F54" s="5">
         <v>7102106</v>
       </c>
-      <c r="G54" s="6" t="s">
-        <v>132</v>
+      <c r="G54" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H54" s="5"/>
-      <c r="I54" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I54" s="5"/>
       <c r="J54" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K54" s="5"/>
-      <c r="L54" s="12"/>
-      <c r="M54" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K54" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L54" s="5"/>
+      <c r="M54" s="11"/>
+      <c r="N54" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="55" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A55" s="5">
         <v>3</v>
       </c>
@@ -3012,23 +3060,24 @@
       <c r="F55" s="5">
         <v>13977776</v>
       </c>
-      <c r="G55" s="6" t="s">
-        <v>132</v>
+      <c r="G55" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H55" s="5"/>
-      <c r="I55" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I55" s="5"/>
       <c r="J55" s="5" t="s">
-        <v>105</v>
-      </c>
-      <c r="K55" s="5"/>
-      <c r="L55" s="12"/>
-      <c r="M55" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+        <v>99</v>
+      </c>
+      <c r="K55" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L55" s="5"/>
+      <c r="M55" s="11"/>
+      <c r="N55" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="56" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A56" s="5">
         <v>3</v>
       </c>
@@ -3047,27 +3096,28 @@
       <c r="F56" s="5">
         <v>130360</v>
       </c>
-      <c r="G56" s="6" t="s">
-        <v>132</v>
+      <c r="G56" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H56" s="5"/>
-      <c r="I56" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I56" s="5"/>
       <c r="J56" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K56" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L56" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M56" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L56" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M56" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N56" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="57" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A57" s="5">
         <v>3</v>
       </c>
@@ -3086,27 +3136,28 @@
       <c r="F57" s="5">
         <v>2117953</v>
       </c>
-      <c r="G57" s="6" t="s">
-        <v>132</v>
+      <c r="G57" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H57" s="5"/>
-      <c r="I57" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I57" s="5"/>
       <c r="J57" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K57" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L57" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M57" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L57" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M57" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N57" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="58" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A58" s="5">
         <v>3</v>
       </c>
@@ -3125,27 +3176,28 @@
       <c r="F58" s="5">
         <v>350076</v>
       </c>
-      <c r="G58" s="6" t="s">
-        <v>132</v>
+      <c r="G58" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H58" s="5"/>
-      <c r="I58" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I58" s="5"/>
       <c r="J58" s="5" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="K58" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="L58" s="5" t="s">
+        <v>111</v>
+      </c>
+      <c r="M58" s="11" t="s">
         <v>112</v>
       </c>
-      <c r="L58" s="12" t="s">
-        <v>113</v>
-      </c>
-      <c r="M58" s="5" t="s">
-        <v>135</v>
-      </c>
-    </row>
-    <row r="59" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N58" s="5" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="59" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A59" s="5">
         <v>3</v>
       </c>
@@ -3164,60 +3216,62 @@
       <c r="F59" s="5">
         <v>23568498</v>
       </c>
-      <c r="G59" s="6" t="s">
-        <v>132</v>
+      <c r="G59" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H59" s="5"/>
-      <c r="I59" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I59" s="5"/>
       <c r="J59" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K59" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L59" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="K59" s="5" t="s">
+      <c r="M59" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L59" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="M59" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
-      <c r="A60" s="10">
-        <v>3</v>
-      </c>
-      <c r="B60" s="10" t="s">
+      <c r="N59" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="60" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A60" s="9">
+        <v>3</v>
+      </c>
+      <c r="B60" s="9" t="s">
         <v>54</v>
       </c>
-      <c r="C60" s="10" t="s">
+      <c r="C60" s="9" t="s">
         <v>58</v>
       </c>
-      <c r="D60" s="10" t="s">
+      <c r="D60" s="9" t="s">
         <v>56</v>
       </c>
-      <c r="E60" s="10" t="s">
+      <c r="E60" s="9" t="s">
         <v>57</v>
       </c>
-      <c r="F60" s="10">
+      <c r="F60" s="9">
         <v>0</v>
       </c>
-      <c r="G60" s="10" t="s">
-        <v>132</v>
-      </c>
-      <c r="H60" s="10"/>
-      <c r="I60" s="10" t="s">
-        <v>100</v>
-      </c>
-      <c r="J60" s="10"/>
-      <c r="K60" s="10"/>
-      <c r="L60" s="16"/>
-      <c r="M60" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="G60" s="9" t="s">
+        <v>131</v>
+      </c>
+      <c r="H60" s="9"/>
+      <c r="I60" s="9"/>
+      <c r="J60" s="9" t="s">
+        <v>99</v>
+      </c>
+      <c r="K60" s="9"/>
+      <c r="L60" s="9"/>
+      <c r="M60" s="15"/>
+      <c r="N60" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="61" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A61" s="5">
         <v>3</v>
       </c>
@@ -3236,27 +3290,28 @@
       <c r="F61" s="5">
         <v>302936543</v>
       </c>
-      <c r="G61" s="6" t="s">
-        <v>132</v>
+      <c r="G61" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H61" s="5"/>
-      <c r="I61" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I61" s="5"/>
       <c r="J61" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K61" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L61" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="K61" s="5" t="s">
+      <c r="M61" s="11" t="s">
         <v>116</v>
       </c>
-      <c r="L61" s="12" t="s">
-        <v>117</v>
-      </c>
-      <c r="M61" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N61" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="62" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A62" s="5">
         <v>3</v>
       </c>
@@ -3275,27 +3330,28 @@
       <c r="F62" s="5">
         <v>4047625</v>
       </c>
-      <c r="G62" s="6" t="s">
-        <v>132</v>
+      <c r="G62" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H62" s="5"/>
-      <c r="I62" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I62" s="5"/>
       <c r="J62" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="K62" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L62" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M62" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="L62" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="M62" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N62" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="63" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A63" s="5">
         <v>3</v>
       </c>
@@ -3314,27 +3370,28 @@
       <c r="F63" s="5">
         <v>189545979</v>
       </c>
-      <c r="G63" s="6" t="s">
-        <v>132</v>
+      <c r="G63" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H63" s="5"/>
-      <c r="I63" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I63" s="5"/>
       <c r="J63" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="K63" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L63" s="5" t="s">
+        <v>119</v>
+      </c>
+      <c r="M63" s="11" t="s">
         <v>120</v>
       </c>
-      <c r="L63" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="M63" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="64" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N63" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A64" s="5">
         <v>3</v>
       </c>
@@ -3353,27 +3410,28 @@
       <c r="F64" s="5">
         <v>74706163</v>
       </c>
-      <c r="G64" s="6" t="s">
-        <v>132</v>
+      <c r="G64" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H64" s="5"/>
-      <c r="I64" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I64" s="5"/>
       <c r="J64" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="K64" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L64" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M64" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="L64" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="M64" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="65" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N64" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="5">
         <v>3</v>
       </c>
@@ -3392,27 +3450,28 @@
       <c r="F65" s="5">
         <v>36660864</v>
       </c>
-      <c r="G65" s="6" t="s">
-        <v>132</v>
+      <c r="G65" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H65" s="5"/>
-      <c r="I65" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I65" s="5"/>
       <c r="J65" s="5" t="s">
-        <v>115</v>
+        <v>99</v>
       </c>
       <c r="K65" s="5" t="s">
+        <v>114</v>
+      </c>
+      <c r="L65" s="5" t="s">
+        <v>117</v>
+      </c>
+      <c r="M65" s="11" t="s">
         <v>118</v>
       </c>
-      <c r="L65" s="12" t="s">
-        <v>119</v>
-      </c>
-      <c r="M65" s="5" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="66" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N65" s="5" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="66" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A66" s="5">
         <v>3</v>
       </c>
@@ -3431,27 +3490,28 @@
       <c r="F66" s="5">
         <v>1141648</v>
       </c>
-      <c r="G66" s="6" t="s">
-        <v>132</v>
+      <c r="G66" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H66" s="5"/>
-      <c r="I66" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I66" s="5"/>
       <c r="J66" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K66" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L66" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K66" s="5" t="s">
+      <c r="M66" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="L66" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="M66" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="67" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N66" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="67" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A67" s="5">
         <v>3</v>
       </c>
@@ -3470,27 +3530,28 @@
       <c r="F67" s="5">
         <v>13879453</v>
       </c>
-      <c r="G67" s="6" t="s">
-        <v>132</v>
+      <c r="G67" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H67" s="5"/>
-      <c r="I67" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I67" s="5"/>
       <c r="J67" s="5" t="s">
-        <v>122</v>
+        <v>99</v>
       </c>
       <c r="K67" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L67" s="5" t="s">
+        <v>124</v>
+      </c>
+      <c r="M67" s="11" t="s">
         <v>125</v>
       </c>
-      <c r="L67" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="M67" s="5" t="s">
-        <v>137</v>
-      </c>
-    </row>
-    <row r="68" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N67" s="5" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="68" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A68" s="5">
         <v>3</v>
       </c>
@@ -3509,27 +3570,28 @@
       <c r="F68" s="5">
         <v>714315</v>
       </c>
-      <c r="G68" s="6" t="s">
-        <v>132</v>
+      <c r="G68" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H68" s="5"/>
-      <c r="I68" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I68" s="5"/>
       <c r="J68" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K68" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L68" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K68" s="5" t="s">
+      <c r="M68" s="11" t="s">
         <v>123</v>
       </c>
-      <c r="L68" s="12" t="s">
-        <v>124</v>
-      </c>
-      <c r="M68" s="5" t="s">
-        <v>139</v>
-      </c>
-    </row>
-    <row r="69" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="N68" s="5" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="69" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A69" s="5">
         <v>3</v>
       </c>
@@ -3548,24 +3610,25 @@
       <c r="F69" s="5">
         <v>498105</v>
       </c>
-      <c r="G69" s="6" t="s">
-        <v>132</v>
+      <c r="G69" s="5" t="s">
+        <v>131</v>
       </c>
       <c r="H69" s="5"/>
-      <c r="I69" s="5" t="s">
-        <v>100</v>
-      </c>
+      <c r="I69" s="5"/>
       <c r="J69" s="5" t="s">
+        <v>99</v>
+      </c>
+      <c r="K69" s="5" t="s">
+        <v>121</v>
+      </c>
+      <c r="L69" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="K69" s="5" t="s">
-        <v>123</v>
-      </c>
-      <c r="L69" s="12" t="s">
-        <v>121</v>
-      </c>
-      <c r="M69" s="5" t="s">
-        <v>139</v>
+      <c r="M69" s="11" t="s">
+        <v>120</v>
+      </c>
+      <c r="N69" s="5" t="s">
+        <v>138</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
feat/calc ready to use
</commit_message>
<xml_diff>
--- a/src/common/bd/DiccionarioMultiX.xlsx
+++ b/src/common/bd/DiccionarioMultiX.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Nicolas Huerta\Documents\nhuerta\Proyectos\zeroco\BackEnd\src\common\bd\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CE93A97-3C75-477F-B610-88B076C23BD4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1367E2A3-CE6D-48C3-B971-2C217A7FF88E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="57480" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{D6A7E3F4-D4FA-4332-B22C-F7F93CCAE935}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21220" xr2:uid="{D6A7E3F4-D4FA-4332-B22C-F7F93CCAE935}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="313">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="944" uniqueCount="312">
   <si>
     <t>Gasolina</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>Fierro</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> </t>
   </si>
   <si>
     <t>Lodos proceso</t>
@@ -1015,7 +1012,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1055,6 +1052,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.79998168889431442"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -1112,7 +1115,7 @@
     <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1171,12 +1174,6 @@
     <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1184,6 +1181,15 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -1504,8 +1510,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7BAD24B2-CCAB-4B33-A88E-76925CA353A4}">
   <dimension ref="A1:N69"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="N2" sqref="N2"/>
+    <sheetView tabSelected="1" topLeftCell="A19" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1529,44 +1535,44 @@
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="D1" s="1" t="s">
         <v>69</v>
       </c>
-      <c r="B1" s="1" t="s">
-        <v>72</v>
-      </c>
-      <c r="C1" s="1" t="s">
+      <c r="E1" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>73</v>
       </c>
-      <c r="D1" s="1" t="s">
-        <v>70</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>71</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>74</v>
-      </c>
       <c r="G1" s="1" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="H1" s="2"/>
       <c r="I1" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="J1" s="1" t="s">
         <v>122</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>123</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="8" t="s">
         <v>124</v>
       </c>
-      <c r="L1" s="8" t="s">
-        <v>125</v>
-      </c>
       <c r="M1" s="1" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="N1" s="1" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
     </row>
     <row r="2" spans="1:14" x14ac:dyDescent="0.35">
@@ -1589,23 +1595,23 @@
         <v>23210</v>
       </c>
       <c r="G2" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J2" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K2" s="4" t="s">
         <v>79</v>
-      </c>
-      <c r="K2" s="4" t="s">
-        <v>80</v>
       </c>
       <c r="L2" s="9" t="s">
         <v>0</v>
       </c>
       <c r="M2" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N2" s="4"/>
     </row>
@@ -1629,23 +1635,23 @@
         <v>3580</v>
       </c>
       <c r="G3" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J3" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J3" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="K3" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L3" s="9" t="s">
         <v>0</v>
       </c>
       <c r="M3" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N3" s="4"/>
     </row>
@@ -1669,23 +1675,23 @@
         <v>1129243</v>
       </c>
       <c r="G4" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J4" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K4" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L4" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N4" s="4"/>
     </row>
@@ -1709,23 +1715,23 @@
         <v>8951</v>
       </c>
       <c r="G5" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J5" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K5" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L5" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M5" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N5" s="4"/>
     </row>
@@ -1749,23 +1755,23 @@
         <v>105022</v>
       </c>
       <c r="G6" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J6" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K6" s="4" t="s">
         <v>7</v>
       </c>
       <c r="L6" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M6" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N6" s="4"/>
     </row>
@@ -1789,23 +1795,23 @@
         <v>21920</v>
       </c>
       <c r="G7" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J7" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J7" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="K7" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L7" s="9" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
       <c r="M7" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N7" s="4"/>
     </row>
@@ -1829,23 +1835,23 @@
         <v>135132</v>
       </c>
       <c r="G8" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J8" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K8" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K8" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="L8" s="9" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="M8" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N8" s="4"/>
     </row>
@@ -1869,23 +1875,23 @@
         <v>700</v>
       </c>
       <c r="G9" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J9" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K9" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K9" s="4" t="s">
+      <c r="L9" s="9" t="s">
         <v>80</v>
       </c>
-      <c r="L9" s="9" t="s">
-        <v>81</v>
-      </c>
       <c r="M9" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N9" s="4"/>
     </row>
@@ -1909,23 +1915,23 @@
         <v>5221203</v>
       </c>
       <c r="G10" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H10" s="4"/>
       <c r="I10" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J10" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J10" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="K10" s="4" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="L10" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M10" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N10" s="4"/>
     </row>
@@ -1949,23 +1955,23 @@
         <v>756989</v>
       </c>
       <c r="G11" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H11" s="4"/>
       <c r="I11" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J11" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K11" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M11" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N11" s="4"/>
     </row>
@@ -1989,23 +1995,23 @@
         <v>3664514</v>
       </c>
       <c r="G12" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H12" s="4"/>
       <c r="I12" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J12" s="4" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="K12" s="4" t="s">
         <v>15</v>
       </c>
       <c r="L12" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M12" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N12" s="4"/>
     </row>
@@ -2029,23 +2035,23 @@
         <v>35600</v>
       </c>
       <c r="G13" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H13" s="4"/>
       <c r="I13" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J13" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K13" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K13" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="L13" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M13" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N13" s="4"/>
     </row>
@@ -2069,23 +2075,23 @@
         <v>240434</v>
       </c>
       <c r="G14" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H14" s="4"/>
       <c r="I14" s="4" t="s">
+        <v>74</v>
+      </c>
+      <c r="J14" s="4" t="s">
         <v>75</v>
       </c>
-      <c r="J14" s="4" t="s">
-        <v>76</v>
-      </c>
       <c r="K14" s="4" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="L14" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M14" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="N14" s="4"/>
     </row>
@@ -2109,61 +2115,61 @@
         <v>1191116</v>
       </c>
       <c r="G15" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H15" s="4"/>
       <c r="I15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J15" s="4" t="s">
+        <v>78</v>
+      </c>
+      <c r="K15" s="4" t="s">
         <v>79</v>
       </c>
-      <c r="K15" s="4" t="s">
-        <v>80</v>
-      </c>
       <c r="L15" s="9" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="M15" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="N15" s="4"/>
+    </row>
+    <row r="16" spans="1:14" s="24" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A16" s="22">
+        <v>1</v>
+      </c>
+      <c r="B16" s="22" t="s">
+        <v>18</v>
+      </c>
+      <c r="C16" s="22" t="s">
+        <v>19</v>
+      </c>
+      <c r="D16" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E16" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F16" s="22">
+        <v>15626</v>
+      </c>
+      <c r="G16" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H16" s="22"/>
+      <c r="I16" s="22" t="s">
+        <v>74</v>
+      </c>
+      <c r="J16" s="22" t="s">
+        <v>83</v>
+      </c>
+      <c r="K16" s="22"/>
+      <c r="L16" s="23"/>
+      <c r="M16" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="N15" s="4"/>
-    </row>
-    <row r="16" spans="1:14" s="26" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A16" s="24">
-        <v>1</v>
-      </c>
-      <c r="B16" s="24" t="s">
-        <v>18</v>
-      </c>
-      <c r="C16" s="24" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E16" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="24">
-        <v>15626</v>
-      </c>
-      <c r="G16" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H16" s="24"/>
-      <c r="I16" s="24" t="s">
-        <v>75</v>
-      </c>
-      <c r="J16" s="24" t="s">
-        <v>84</v>
-      </c>
-      <c r="K16" s="24"/>
-      <c r="L16" s="25"/>
-      <c r="M16" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N16" s="24">
+      <c r="N16" s="22">
         <v>1810</v>
       </c>
     </row>
@@ -2187,23 +2193,23 @@
         <v>709</v>
       </c>
       <c r="G17" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H17" s="4"/>
       <c r="I17" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J17" s="4" t="s">
+        <v>83</v>
+      </c>
+      <c r="K17" s="4" t="s">
         <v>84</v>
       </c>
-      <c r="K17" s="4" t="s">
-        <v>85</v>
-      </c>
       <c r="L17" s="9" t="s">
-        <v>85</v>
-      </c>
-      <c r="M17" s="22" t="s">
-        <v>130</v>
+        <v>84</v>
+      </c>
+      <c r="M17" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="N17" s="4"/>
     </row>
@@ -2227,23 +2233,23 @@
         <v>90</v>
       </c>
       <c r="G18" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H18" s="4"/>
       <c r="I18" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J18" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K18" s="4" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="L18" s="9" t="s">
-        <v>86</v>
-      </c>
-      <c r="M18" s="22" t="s">
-        <v>130</v>
+        <v>85</v>
+      </c>
+      <c r="M18" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="N18" s="4"/>
     </row>
@@ -2267,223 +2273,223 @@
         <v>136</v>
       </c>
       <c r="G19" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H19" s="4"/>
       <c r="I19" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="J19" s="4" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="K19" s="4" t="s">
+        <v>86</v>
+      </c>
+      <c r="L19" s="9" t="s">
+        <v>86</v>
+      </c>
+      <c r="M19" s="4" t="s">
+        <v>129</v>
+      </c>
+      <c r="N19" s="4"/>
+    </row>
+    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A20" s="4">
+        <v>2</v>
+      </c>
+      <c r="B20" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C20" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="D20" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E20" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F20" s="4">
+        <v>27914</v>
+      </c>
+      <c r="G20" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H20" s="4"/>
+      <c r="I20" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="L19" s="9" t="s">
+      <c r="J20" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K20" s="4" t="s">
+        <v>89</v>
+      </c>
+      <c r="L20" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M20" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N20" s="4"/>
+    </row>
+    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A21" s="4">
+        <v>2</v>
+      </c>
+      <c r="B21" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="D21" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="E21" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F21" s="4">
+        <v>26738</v>
+      </c>
+      <c r="G21" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H21" s="4"/>
+      <c r="I21" s="4" t="s">
         <v>87</v>
       </c>
-      <c r="M19" s="22" t="s">
+      <c r="J21" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K21" s="4" t="s">
+        <v>91</v>
+      </c>
+      <c r="L21" s="9" t="s">
+        <v>90</v>
+      </c>
+      <c r="M21" s="4" t="s">
         <v>130</v>
       </c>
-      <c r="N19" s="4"/>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A20" s="22">
+      <c r="N21" s="4"/>
+    </row>
+    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A22" s="4">
         <v>2</v>
       </c>
-      <c r="B20" s="22" t="s">
+      <c r="B22" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C20" s="22" t="s">
-        <v>25</v>
-      </c>
-      <c r="D20" s="22" t="s">
+      <c r="C22" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D22" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E22" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F22" s="4">
+        <v>4525740</v>
+      </c>
+      <c r="G22" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H22" s="4"/>
+      <c r="I22" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J22" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K22" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L22" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M22" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N22" s="4"/>
+    </row>
+    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A23" s="4">
+        <v>2</v>
+      </c>
+      <c r="B23" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D23" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E23" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="4">
+        <v>35683</v>
+      </c>
+      <c r="G23" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H23" s="4"/>
+      <c r="I23" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J23" s="4" t="s">
+        <v>88</v>
+      </c>
+      <c r="K23" s="4" t="s">
+        <v>92</v>
+      </c>
+      <c r="L23" s="9" t="s">
+        <v>93</v>
+      </c>
+      <c r="M23" s="4" t="s">
+        <v>130</v>
+      </c>
+      <c r="N23" s="4"/>
+    </row>
+    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A24" s="4">
+        <v>2</v>
+      </c>
+      <c r="B24" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E20" s="22" t="s">
+      <c r="E24" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F20" s="22">
-        <v>27914</v>
-      </c>
-      <c r="G20" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H20" s="22"/>
-      <c r="I20" s="22" t="s">
+      <c r="F24" s="4">
+        <v>21344</v>
+      </c>
+      <c r="G24" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H24" s="4"/>
+      <c r="I24" s="4" t="s">
+        <v>87</v>
+      </c>
+      <c r="J24" s="4" t="s">
         <v>88</v>
       </c>
-      <c r="J20" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K20" s="22" t="s">
-        <v>90</v>
-      </c>
-      <c r="L20" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="M20" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="N20" s="4"/>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A21" s="22">
-        <v>2</v>
-      </c>
-      <c r="B21" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C21" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E21" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F21" s="22">
-        <v>26738</v>
-      </c>
-      <c r="G21" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H21" s="22"/>
-      <c r="I21" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="J21" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K21" s="22" t="s">
+      <c r="K24" s="4" t="s">
         <v>92</v>
       </c>
-      <c r="L21" s="23" t="s">
-        <v>91</v>
-      </c>
-      <c r="M21" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="N21" s="4"/>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A22" s="22">
-        <v>2</v>
-      </c>
-      <c r="B22" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C22" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D22" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E22" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F22" s="22">
-        <v>4525740</v>
-      </c>
-      <c r="G22" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H22" s="22"/>
-      <c r="I22" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="J22" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K22" s="22" t="s">
+      <c r="L24" s="9" t="s">
         <v>93</v>
       </c>
-      <c r="L22" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="M22" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="N22" s="4"/>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A23" s="22">
-        <v>2</v>
-      </c>
-      <c r="B23" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C23" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D23" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E23" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F23" s="22">
-        <v>35683</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H23" s="22"/>
-      <c r="I23" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="J23" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K23" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="L23" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="M23" s="22" t="s">
-        <v>131</v>
-      </c>
-      <c r="N23" s="4"/>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A24" s="22">
-        <v>2</v>
-      </c>
-      <c r="B24" s="22" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="22" t="s">
-        <v>28</v>
-      </c>
-      <c r="D24" s="22" t="s">
-        <v>5</v>
-      </c>
-      <c r="E24" s="22" t="s">
-        <v>26</v>
-      </c>
-      <c r="F24" s="22">
-        <v>21344</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H24" s="22"/>
-      <c r="I24" s="22" t="s">
-        <v>88</v>
-      </c>
-      <c r="J24" s="22" t="s">
-        <v>89</v>
-      </c>
-      <c r="K24" s="22" t="s">
-        <v>93</v>
-      </c>
-      <c r="L24" s="23" t="s">
-        <v>94</v>
-      </c>
-      <c r="M24" s="22" t="s">
-        <v>131</v>
+      <c r="M24" s="4" t="s">
+        <v>130</v>
       </c>
       <c r="N24" s="4"/>
     </row>
@@ -2507,137 +2513,137 @@
         <v>16327818</v>
       </c>
       <c r="G25" s="6" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H25" s="6"/>
       <c r="I25" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="J25" s="6"/>
       <c r="K25" s="6"/>
       <c r="L25" s="10"/>
       <c r="M25" s="5" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="N25" s="5"/>
     </row>
     <row r="26" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A26" s="22">
-        <v>3</v>
-      </c>
-      <c r="B26" s="22" t="s">
+      <c r="A26" s="4">
+        <v>3</v>
+      </c>
+      <c r="B26" s="4" t="s">
         <v>30</v>
       </c>
-      <c r="C26" s="22" t="s">
+      <c r="C26" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D26" s="22" t="s">
+      <c r="D26" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E26" s="22" t="s">
+      <c r="E26" s="4" t="s">
         <v>32</v>
       </c>
-      <c r="F26" s="22">
+      <c r="F26" s="4">
         <v>22773</v>
       </c>
-      <c r="G26" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H26" s="22"/>
-      <c r="I26" s="22" t="s">
+      <c r="G26" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="I26" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J26" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J26" s="22" t="s">
+      <c r="K26" s="4" t="s">
         <v>96</v>
       </c>
-      <c r="K26" s="22" t="s">
+      <c r="L26" s="9" t="s">
         <v>97</v>
       </c>
-      <c r="L26" s="23" t="s">
+      <c r="M26" s="4" t="s">
+        <v>128</v>
+      </c>
+      <c r="N26" s="4"/>
+    </row>
+    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A27" s="4">
+        <v>3</v>
+      </c>
+      <c r="B27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="C27" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D27" s="4" t="s">
+        <v>8</v>
+      </c>
+      <c r="E27" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="F27" s="4">
+        <v>4203498</v>
+      </c>
+      <c r="G27" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H27" s="4"/>
+      <c r="I27" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J27" s="4" t="s">
+        <v>95</v>
+      </c>
+      <c r="K27" s="4" t="s">
+        <v>33</v>
+      </c>
+      <c r="L27" s="9" t="s">
         <v>98</v>
       </c>
-      <c r="M26" s="22" t="s">
+      <c r="M27" s="4" t="s">
         <v>129</v>
       </c>
-      <c r="N26" s="4"/>
-    </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A27" s="22">
-        <v>3</v>
-      </c>
-      <c r="B27" s="22" t="s">
+      <c r="N27" s="4"/>
+    </row>
+    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A28" s="4">
+        <v>3</v>
+      </c>
+      <c r="B28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="C27" s="22" t="s">
-        <v>34</v>
-      </c>
-      <c r="D27" s="22" t="s">
-        <v>8</v>
-      </c>
-      <c r="E27" s="22" t="s">
+      <c r="C28" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="D28" s="4" t="s">
+        <v>2</v>
+      </c>
+      <c r="E28" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="F27" s="22">
-        <v>4203498</v>
-      </c>
-      <c r="G27" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H27" s="22"/>
-      <c r="I27" s="22" t="s">
+      <c r="F28" s="4">
+        <v>119043744</v>
+      </c>
+      <c r="G28" s="4" t="s">
+        <v>126</v>
+      </c>
+      <c r="H28" s="4"/>
+      <c r="I28" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="J28" s="4" t="s">
         <v>95</v>
       </c>
-      <c r="J27" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="K27" s="22" t="s">
+      <c r="K28" s="4" t="s">
         <v>33</v>
       </c>
-      <c r="L27" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="M27" s="22" t="s">
-        <v>130</v>
-      </c>
-      <c r="N27" s="4"/>
-    </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A28" s="22">
-        <v>3</v>
-      </c>
-      <c r="B28" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="C28" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="D28" s="22" t="s">
-        <v>2</v>
-      </c>
-      <c r="E28" s="22" t="s">
-        <v>20</v>
-      </c>
-      <c r="F28" s="22">
-        <v>119043744</v>
-      </c>
-      <c r="G28" s="22" t="s">
-        <v>127</v>
-      </c>
-      <c r="H28" s="22"/>
-      <c r="I28" s="22" t="s">
-        <v>95</v>
-      </c>
-      <c r="J28" s="22" t="s">
-        <v>96</v>
-      </c>
-      <c r="K28" s="22" t="s">
-        <v>33</v>
-      </c>
-      <c r="L28" s="23" t="s">
-        <v>99</v>
-      </c>
-      <c r="M28" s="22" t="s">
-        <v>130</v>
+      <c r="L28" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="M28" s="4" t="s">
+        <v>129</v>
       </c>
       <c r="N28" s="4"/>
     </row>
@@ -2661,17 +2667,17 @@
         <v>2517</v>
       </c>
       <c r="G29" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H29" s="7"/>
       <c r="I29" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J29" s="7"/>
       <c r="K29" s="7"/>
       <c r="L29" s="11"/>
       <c r="M29" s="7" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N29" s="7"/>
     </row>
@@ -2695,17 +2701,17 @@
         <v>0</v>
       </c>
       <c r="G30" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H30" s="7"/>
       <c r="I30" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J30" s="7"/>
       <c r="K30" s="7"/>
       <c r="L30" s="11"/>
       <c r="M30" s="7" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N30" s="7"/>
     </row>
@@ -2729,23 +2735,23 @@
         <v>23308</v>
       </c>
       <c r="G31" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H31" s="4"/>
       <c r="I31" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J31" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K31" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K31" s="4" t="s">
+      <c r="L31" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L31" s="9" t="s">
-        <v>102</v>
-      </c>
       <c r="M31" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N31" s="4"/>
     </row>
@@ -2769,23 +2775,23 @@
         <v>212000</v>
       </c>
       <c r="G32" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H32" s="4"/>
       <c r="I32" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J32" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K32" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K32" s="4" t="s">
+      <c r="L32" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="L32" s="9" t="s">
-        <v>102</v>
-      </c>
       <c r="M32" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N32" s="4"/>
     </row>
@@ -2809,23 +2815,23 @@
         <v>5470</v>
       </c>
       <c r="G33" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H33" s="4"/>
       <c r="I33" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J33" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K33" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K33" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L33" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M33" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N33" s="4"/>
     </row>
@@ -2849,17 +2855,17 @@
         <v>0</v>
       </c>
       <c r="G34" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H34" s="7"/>
       <c r="I34" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J34" s="7"/>
       <c r="K34" s="7"/>
       <c r="L34" s="11"/>
       <c r="M34" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N34" s="11"/>
     </row>
@@ -2883,23 +2889,23 @@
         <v>32984</v>
       </c>
       <c r="G35" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H35" s="4"/>
       <c r="I35" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J35" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K35" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K35" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L35" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M35" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N35" s="4"/>
     </row>
@@ -2923,23 +2929,23 @@
         <v>3100</v>
       </c>
       <c r="G36" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H36" s="4"/>
       <c r="I36" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J36" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K36" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K36" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L36" s="9" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="M36" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N36" s="4"/>
     </row>
@@ -2963,65 +2969,65 @@
         <v>5000</v>
       </c>
       <c r="G37" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H37" s="4"/>
       <c r="I37" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J37" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K37" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K37" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L37" s="9" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="M37" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N37" s="4"/>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A38" s="4">
-        <v>3</v>
-      </c>
-      <c r="B38" s="4" t="s">
+    <row r="38" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A38" s="25">
+        <v>3</v>
+      </c>
+      <c r="B38" s="25" t="s">
         <v>39</v>
       </c>
-      <c r="C38" s="4" t="s">
+      <c r="C38" s="25" t="s">
         <v>44</v>
       </c>
-      <c r="D38" s="4" t="s">
+      <c r="D38" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="E38" s="4" t="s">
+      <c r="E38" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="F38" s="4">
+      <c r="F38" s="25">
         <v>1871000</v>
       </c>
-      <c r="G38" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H38" s="4"/>
-      <c r="I38" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J38" s="4" t="s">
-        <v>100</v>
-      </c>
-      <c r="K38" s="4" t="s">
+      <c r="G38" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H38" s="25"/>
+      <c r="I38" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="K38" s="25" t="s">
+        <v>104</v>
+      </c>
+      <c r="L38" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="L38" s="9" t="s">
-        <v>106</v>
-      </c>
-      <c r="M38" s="4" t="s">
-        <v>130</v>
-      </c>
-      <c r="N38" s="4"/>
+      <c r="M38" s="25" t="s">
+        <v>129</v>
+      </c>
+      <c r="N38" s="25"/>
     </row>
     <row r="39" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A39" s="7">
@@ -3031,7 +3037,7 @@
         <v>39</v>
       </c>
       <c r="C39" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D39" s="7" t="s">
         <v>2</v>
@@ -3043,17 +3049,17 @@
         <v>0</v>
       </c>
       <c r="G39" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H39" s="7"/>
       <c r="I39" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J39" s="7"/>
       <c r="K39" s="7"/>
       <c r="L39" s="11"/>
       <c r="M39" s="11" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N39" s="11"/>
     </row>
@@ -3065,7 +3071,7 @@
         <v>39</v>
       </c>
       <c r="C40" s="4" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="D40" s="4" t="s">
         <v>9</v>
@@ -3077,23 +3083,23 @@
         <v>1435000</v>
       </c>
       <c r="G40" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H40" s="4"/>
       <c r="I40" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J40" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K40" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="L40" s="9" t="s">
         <v>105</v>
       </c>
-      <c r="L40" s="9" t="s">
-        <v>106</v>
-      </c>
       <c r="M40" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N40" s="4"/>
     </row>
@@ -3105,7 +3111,7 @@
         <v>39</v>
       </c>
       <c r="C41" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D41" s="4" t="s">
         <v>8</v>
@@ -3117,23 +3123,23 @@
         <v>38000</v>
       </c>
       <c r="G41" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H41" s="4"/>
       <c r="I41" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J41" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K41" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L41" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L41" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="M41" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N41" s="4"/>
     </row>
@@ -3145,7 +3151,7 @@
         <v>39</v>
       </c>
       <c r="C42" s="4" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="D42" s="4" t="s">
         <v>2</v>
@@ -3157,23 +3163,23 @@
         <v>21599</v>
       </c>
       <c r="G42" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H42" s="4"/>
       <c r="I42" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J42" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K42" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L42" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L42" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="M42" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N42" s="4"/>
     </row>
@@ -3185,7 +3191,7 @@
         <v>39</v>
       </c>
       <c r="C43" s="4" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="D43" s="4" t="s">
         <v>2</v>
@@ -3197,23 +3203,23 @@
         <v>46584</v>
       </c>
       <c r="G43" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H43" s="4"/>
       <c r="I43" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J43" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K43" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K43" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L43" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M43" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N43" s="4"/>
     </row>
@@ -3225,7 +3231,7 @@
         <v>39</v>
       </c>
       <c r="C44" s="4" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="D44" s="4" t="s">
         <v>2</v>
@@ -3237,213 +3243,213 @@
         <v>697475</v>
       </c>
       <c r="G44" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H44" s="4"/>
       <c r="I44" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J44" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K44" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K44" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L44" s="9" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="M44" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N44" s="4"/>
     </row>
     <row r="45" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A45" s="24">
-        <v>3</v>
-      </c>
-      <c r="B45" s="24" t="s">
+      <c r="A45" s="22">
+        <v>3</v>
+      </c>
+      <c r="B45" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C45" s="24" t="s">
+      <c r="C45" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D45" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E45" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F45" s="22">
+        <v>176231</v>
+      </c>
+      <c r="G45" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H45" s="22"/>
+      <c r="I45" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J45" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K45" s="22"/>
+      <c r="L45" s="23"/>
+      <c r="M45" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N45" s="22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A46" s="22">
+        <v>3</v>
+      </c>
+      <c r="B46" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C46" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D46" s="22" t="s">
+        <v>9</v>
+      </c>
+      <c r="E46" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F46" s="22">
+        <v>7620</v>
+      </c>
+      <c r="G46" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H46" s="22"/>
+      <c r="I46" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J46" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K46" s="22"/>
+      <c r="L46" s="23"/>
+      <c r="M46" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N46" s="22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A47" s="22">
+        <v>3</v>
+      </c>
+      <c r="B47" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C47" s="22" t="s">
+        <v>48</v>
+      </c>
+      <c r="D47" s="22" t="s">
+        <v>2</v>
+      </c>
+      <c r="E47" s="22" t="s">
+        <v>20</v>
+      </c>
+      <c r="F47" s="22">
+        <v>138</v>
+      </c>
+      <c r="G47" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H47" s="22"/>
+      <c r="I47" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J47" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K47" s="22"/>
+      <c r="L47" s="23"/>
+      <c r="M47" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N47" s="22">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A48" s="22">
+        <v>3</v>
+      </c>
+      <c r="B48" s="22" t="s">
+        <v>39</v>
+      </c>
+      <c r="C48" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D45" s="24" t="s">
+      <c r="D48" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E45" s="24" t="s">
+      <c r="E48" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F45" s="24">
-        <v>176231</v>
-      </c>
-      <c r="G45" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H45" s="24"/>
-      <c r="I45" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J45" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K45" s="24"/>
-      <c r="L45" s="25"/>
-      <c r="M45" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N45" s="24">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A46" s="24">
-        <v>3</v>
-      </c>
-      <c r="B46" s="24" t="s">
+      <c r="F48" s="22">
+        <v>18482</v>
+      </c>
+      <c r="G48" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H48" s="22"/>
+      <c r="I48" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J48" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K48" s="22"/>
+      <c r="L48" s="23"/>
+      <c r="M48" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N48" s="22">
+        <v>2000</v>
+      </c>
+    </row>
+    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
+      <c r="A49" s="22">
+        <v>3</v>
+      </c>
+      <c r="B49" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C46" s="24" t="s">
+      <c r="C49" s="22" t="s">
         <v>49</v>
       </c>
-      <c r="D46" s="24" t="s">
+      <c r="D49" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E46" s="24" t="s">
+      <c r="E49" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F46" s="24">
-        <v>7620</v>
-      </c>
-      <c r="G46" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H46" s="24"/>
-      <c r="I46" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J46" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K46" s="24"/>
-      <c r="L46" s="25"/>
-      <c r="M46" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N46" s="24">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A47" s="24">
-        <v>3</v>
-      </c>
-      <c r="B47" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C47" s="24" t="s">
-        <v>49</v>
-      </c>
-      <c r="D47" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E47" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F47" s="24">
-        <v>138</v>
-      </c>
-      <c r="G47" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H47" s="24"/>
-      <c r="I47" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J47" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K47" s="24"/>
-      <c r="L47" s="25"/>
-      <c r="M47" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N47" s="24">
-        <v>400</v>
-      </c>
-    </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A48" s="24">
-        <v>3</v>
-      </c>
-      <c r="B48" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C48" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D48" s="24" t="s">
-        <v>2</v>
-      </c>
-      <c r="E48" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F48" s="24">
-        <v>18482</v>
-      </c>
-      <c r="G48" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H48" s="24"/>
-      <c r="I48" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J48" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K48" s="24"/>
-      <c r="L48" s="25"/>
-      <c r="M48" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N48" s="24">
-        <v>2000</v>
-      </c>
-    </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A49" s="24">
-        <v>3</v>
-      </c>
-      <c r="B49" s="24" t="s">
-        <v>39</v>
-      </c>
-      <c r="C49" s="24" t="s">
-        <v>50</v>
-      </c>
-      <c r="D49" s="24" t="s">
-        <v>9</v>
-      </c>
-      <c r="E49" s="24" t="s">
-        <v>20</v>
-      </c>
-      <c r="F49" s="24">
+      <c r="F49" s="22">
         <v>493</v>
       </c>
-      <c r="G49" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H49" s="24"/>
-      <c r="I49" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J49" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K49" s="24"/>
-      <c r="L49" s="25"/>
-      <c r="M49" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N49" s="24">
+      <c r="G49" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H49" s="22"/>
+      <c r="I49" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J49" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K49" s="22"/>
+      <c r="L49" s="23"/>
+      <c r="M49" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N49" s="22">
         <v>2000</v>
       </c>
     </row>
@@ -3455,7 +3461,7 @@
         <v>39</v>
       </c>
       <c r="C50" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D50" s="4" t="s">
         <v>8</v>
@@ -3467,23 +3473,23 @@
         <v>10463</v>
       </c>
       <c r="G50" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H50" s="4"/>
       <c r="I50" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J50" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K50" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K50" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L50" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M50" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N50" s="4"/>
     </row>
@@ -3495,7 +3501,7 @@
         <v>39</v>
       </c>
       <c r="C51" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D51" s="4" t="s">
         <v>2</v>
@@ -3507,23 +3513,23 @@
         <v>408687</v>
       </c>
       <c r="G51" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H51" s="4"/>
       <c r="I51" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J51" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K51" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K51" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L51" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M51" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N51" s="4"/>
     </row>
@@ -3535,7 +3541,7 @@
         <v>39</v>
       </c>
       <c r="C52" s="4" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="D52" s="4" t="s">
         <v>9</v>
@@ -3547,137 +3553,137 @@
         <v>164080</v>
       </c>
       <c r="G52" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H52" s="4"/>
       <c r="I52" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J52" s="4" t="s">
+        <v>99</v>
+      </c>
+      <c r="K52" s="4" t="s">
         <v>100</v>
       </c>
-      <c r="K52" s="4" t="s">
-        <v>101</v>
-      </c>
       <c r="L52" s="9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="M52" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N52" s="4"/>
     </row>
     <row r="53" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A53" s="24">
-        <v>3</v>
-      </c>
-      <c r="B53" s="24" t="s">
+      <c r="A53" s="22">
+        <v>3</v>
+      </c>
+      <c r="B53" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C53" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D53" s="24" t="s">
+      <c r="C53" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D53" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="E53" s="24" t="s">
+      <c r="E53" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F53" s="24">
+      <c r="F53" s="22">
         <v>491610</v>
       </c>
-      <c r="G53" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H53" s="24"/>
-      <c r="I53" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J53" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K53" s="24"/>
-      <c r="L53" s="25"/>
-      <c r="M53" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N53" s="24">
+      <c r="G53" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H53" s="22"/>
+      <c r="I53" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J53" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K53" s="22"/>
+      <c r="L53" s="23"/>
+      <c r="M53" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N53" s="22">
         <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A54" s="24">
-        <v>3</v>
-      </c>
-      <c r="B54" s="24" t="s">
+      <c r="A54" s="22">
+        <v>3</v>
+      </c>
+      <c r="B54" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C54" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D54" s="24" t="s">
+      <c r="C54" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D54" s="22" t="s">
         <v>2</v>
       </c>
-      <c r="E54" s="24" t="s">
+      <c r="E54" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F54" s="24">
+      <c r="F54" s="22">
         <v>7102106</v>
       </c>
-      <c r="G54" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H54" s="24"/>
-      <c r="I54" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J54" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K54" s="24"/>
-      <c r="L54" s="25"/>
-      <c r="M54" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N54" s="24">
+      <c r="G54" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H54" s="22"/>
+      <c r="I54" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J54" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K54" s="22"/>
+      <c r="L54" s="23"/>
+      <c r="M54" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N54" s="22">
         <v>20</v>
       </c>
     </row>
     <row r="55" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A55" s="24">
-        <v>3</v>
-      </c>
-      <c r="B55" s="24" t="s">
+      <c r="A55" s="22">
+        <v>3</v>
+      </c>
+      <c r="B55" s="22" t="s">
         <v>39</v>
       </c>
-      <c r="C55" s="24" t="s">
-        <v>52</v>
-      </c>
-      <c r="D55" s="24" t="s">
+      <c r="C55" s="22" t="s">
+        <v>51</v>
+      </c>
+      <c r="D55" s="22" t="s">
         <v>9</v>
       </c>
-      <c r="E55" s="24" t="s">
+      <c r="E55" s="22" t="s">
         <v>20</v>
       </c>
-      <c r="F55" s="24">
+      <c r="F55" s="22">
         <v>13977776</v>
       </c>
-      <c r="G55" s="24" t="s">
-        <v>127</v>
-      </c>
-      <c r="H55" s="24"/>
-      <c r="I55" s="24" t="s">
-        <v>95</v>
-      </c>
-      <c r="J55" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="K55" s="24"/>
-      <c r="L55" s="25"/>
-      <c r="M55" s="24" t="s">
-        <v>130</v>
-      </c>
-      <c r="N55" s="24">
+      <c r="G55" s="22" t="s">
+        <v>126</v>
+      </c>
+      <c r="H55" s="22"/>
+      <c r="I55" s="22" t="s">
+        <v>94</v>
+      </c>
+      <c r="J55" s="22" t="s">
+        <v>99</v>
+      </c>
+      <c r="K55" s="22"/>
+      <c r="L55" s="23"/>
+      <c r="M55" s="22" t="s">
+        <v>129</v>
+      </c>
+      <c r="N55" s="22">
         <v>20</v>
       </c>
     </row>
@@ -3689,7 +3695,7 @@
         <v>39</v>
       </c>
       <c r="C56" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D56" s="4" t="s">
         <v>8</v>
@@ -3701,23 +3707,23 @@
         <v>130360</v>
       </c>
       <c r="G56" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H56" s="4"/>
       <c r="I56" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J56" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K56" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L56" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L56" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="M56" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N56" s="4"/>
     </row>
@@ -3729,7 +3735,7 @@
         <v>39</v>
       </c>
       <c r="C57" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D57" s="4" t="s">
         <v>2</v>
@@ -3741,23 +3747,23 @@
         <v>2117953</v>
       </c>
       <c r="G57" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H57" s="4"/>
       <c r="I57" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J57" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K57" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L57" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L57" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="M57" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N57" s="4"/>
     </row>
@@ -3769,7 +3775,7 @@
         <v>39</v>
       </c>
       <c r="C58" s="4" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D58" s="4" t="s">
         <v>9</v>
@@ -3781,23 +3787,23 @@
         <v>350076</v>
       </c>
       <c r="G58" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H58" s="4"/>
       <c r="I58" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J58" s="4" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="K58" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="L58" s="9" t="s">
         <v>107</v>
       </c>
-      <c r="L58" s="9" t="s">
-        <v>108</v>
-      </c>
       <c r="M58" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="N58" s="4"/>
     </row>
@@ -3806,38 +3812,38 @@
         <v>3</v>
       </c>
       <c r="B59" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="C59" s="4" t="s">
         <v>54</v>
       </c>
-      <c r="C59" s="4" t="s">
+      <c r="D59" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D59" s="4" t="s">
+      <c r="E59" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E59" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="F59" s="4">
         <v>23568498</v>
       </c>
       <c r="G59" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H59" s="4"/>
       <c r="I59" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J59" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K59" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K59" s="4" t="s">
+      <c r="L59" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L59" s="9" t="s">
-        <v>112</v>
-      </c>
       <c r="M59" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N59" s="4"/>
     </row>
@@ -3846,32 +3852,32 @@
         <v>3</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="C60" s="7" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D60" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E60" s="7" t="s">
         <v>56</v>
-      </c>
-      <c r="E60" s="7" t="s">
-        <v>57</v>
       </c>
       <c r="F60" s="7">
         <v>0</v>
       </c>
       <c r="G60" s="7" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H60" s="7"/>
       <c r="I60" s="7" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J60" s="7"/>
       <c r="K60" s="7"/>
       <c r="L60" s="11"/>
       <c r="M60" s="11" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N60" s="11"/>
     </row>
@@ -3880,38 +3886,38 @@
         <v>3</v>
       </c>
       <c r="B61" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C61" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="D61" s="4" t="s">
         <v>55</v>
       </c>
-      <c r="D61" s="4" t="s">
+      <c r="E61" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E61" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="F61" s="4">
         <v>302936543</v>
       </c>
       <c r="G61" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H61" s="4"/>
       <c r="I61" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J61" s="4" t="s">
+        <v>109</v>
+      </c>
+      <c r="K61" s="4" t="s">
         <v>110</v>
       </c>
-      <c r="K61" s="4" t="s">
+      <c r="L61" s="9" t="s">
         <v>111</v>
       </c>
-      <c r="L61" s="9" t="s">
-        <v>112</v>
-      </c>
       <c r="M61" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N61" s="4"/>
     </row>
@@ -3920,38 +3926,38 @@
         <v>3</v>
       </c>
       <c r="B62" s="4" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C62" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D62" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E62" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E62" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="F62" s="4">
         <v>4047625</v>
       </c>
       <c r="G62" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H62" s="4"/>
       <c r="I62" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J62" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K62" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L62" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="L62" s="9" t="s">
-        <v>114</v>
-      </c>
       <c r="M62" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N62" s="4"/>
     </row>
@@ -3960,118 +3966,118 @@
         <v>3</v>
       </c>
       <c r="B63" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="C63" s="4" t="s">
         <v>60</v>
       </c>
-      <c r="C63" s="4" t="s">
-        <v>61</v>
-      </c>
       <c r="D63" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E63" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E63" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="F63" s="4">
         <v>189545979</v>
       </c>
       <c r="G63" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H63" s="4"/>
       <c r="I63" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J63" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K63" s="4" t="s">
+        <v>114</v>
+      </c>
+      <c r="L63" s="9" t="s">
         <v>115</v>
       </c>
-      <c r="L63" s="9" t="s">
-        <v>116</v>
-      </c>
       <c r="M63" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N63" s="4"/>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.35">
-      <c r="A64" s="4">
-        <v>3</v>
-      </c>
-      <c r="B64" s="4" t="s">
+    <row r="64" spans="1:14" s="27" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A64" s="25">
+        <v>3</v>
+      </c>
+      <c r="B64" s="25" t="s">
+        <v>59</v>
+      </c>
+      <c r="C64" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C64" s="4" t="s">
-        <v>61</v>
-      </c>
-      <c r="D64" s="4" t="s">
+      <c r="D64" s="25" t="s">
+        <v>55</v>
+      </c>
+      <c r="E64" s="25" t="s">
         <v>56</v>
       </c>
-      <c r="E64" s="4" t="s">
-        <v>57</v>
-      </c>
-      <c r="F64" s="4">
+      <c r="F64" s="25">
         <v>74706163</v>
       </c>
-      <c r="G64" s="4" t="s">
-        <v>127</v>
-      </c>
-      <c r="H64" s="4"/>
-      <c r="I64" s="4" t="s">
-        <v>95</v>
-      </c>
-      <c r="J64" s="4" t="s">
-        <v>110</v>
-      </c>
-      <c r="K64" s="4" t="s">
+      <c r="G64" s="25" t="s">
+        <v>126</v>
+      </c>
+      <c r="H64" s="25"/>
+      <c r="I64" s="25" t="s">
+        <v>94</v>
+      </c>
+      <c r="J64" s="25" t="s">
+        <v>109</v>
+      </c>
+      <c r="K64" s="25" t="s">
+        <v>112</v>
+      </c>
+      <c r="L64" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="L64" s="9" t="s">
-        <v>114</v>
-      </c>
-      <c r="M64" s="4" t="s">
-        <v>133</v>
-      </c>
-      <c r="N64" s="4"/>
+      <c r="M64" s="25" t="s">
+        <v>132</v>
+      </c>
+      <c r="N64" s="25"/>
     </row>
     <row r="65" spans="1:14" x14ac:dyDescent="0.35">
       <c r="A65" s="4">
         <v>3</v>
       </c>
       <c r="B65" s="4" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="C65" s="4" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="D65" s="4" t="s">
+        <v>55</v>
+      </c>
+      <c r="E65" s="4" t="s">
         <v>56</v>
-      </c>
-      <c r="E65" s="4" t="s">
-        <v>57</v>
       </c>
       <c r="F65" s="4">
         <v>36660864</v>
       </c>
       <c r="G65" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H65" s="4"/>
       <c r="I65" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J65" s="4" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="K65" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="L65" s="9" t="s">
         <v>113</v>
       </c>
-      <c r="L65" s="9" t="s">
-        <v>114</v>
-      </c>
       <c r="M65" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="N65" s="4"/>
     </row>
@@ -4080,7 +4086,7 @@
         <v>3</v>
       </c>
       <c r="B66" s="4" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="C66" s="4" t="s">
         <v>37</v>
@@ -4089,29 +4095,29 @@
         <v>2</v>
       </c>
       <c r="E66" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F66" s="4">
         <v>1141648</v>
       </c>
       <c r="G66" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H66" s="4"/>
       <c r="I66" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J66" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K66" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K66" s="4" t="s">
+      <c r="L66" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="L66" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="M66" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N66" s="4"/>
     </row>
@@ -4120,7 +4126,7 @@
         <v>3</v>
       </c>
       <c r="B67" s="4" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="C67" s="4" t="s">
         <v>37</v>
@@ -4135,23 +4141,23 @@
         <v>13879453</v>
       </c>
       <c r="G67" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H67" s="4"/>
       <c r="I67" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J67" s="4" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="K67" s="4" t="s">
+        <v>119</v>
+      </c>
+      <c r="L67" s="9" t="s">
         <v>120</v>
       </c>
-      <c r="L67" s="9" t="s">
-        <v>121</v>
-      </c>
       <c r="M67" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="N67" s="4"/>
     </row>
@@ -4160,7 +4166,7 @@
         <v>3</v>
       </c>
       <c r="B68" s="4" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C68" s="4" t="s">
         <v>37</v>
@@ -4169,29 +4175,29 @@
         <v>2</v>
       </c>
       <c r="E68" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F68" s="4">
         <v>714315</v>
       </c>
       <c r="G68" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H68" s="4"/>
       <c r="I68" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J68" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K68" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K68" s="4" t="s">
+      <c r="L68" s="9" t="s">
         <v>118</v>
       </c>
-      <c r="L68" s="9" t="s">
-        <v>119</v>
-      </c>
       <c r="M68" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N68" s="4"/>
     </row>
@@ -4200,38 +4206,38 @@
         <v>3</v>
       </c>
       <c r="B69" s="4" t="s">
+        <v>66</v>
+      </c>
+      <c r="C69" s="4" t="s">
         <v>67</v>
-      </c>
-      <c r="C69" s="4" t="s">
-        <v>68</v>
       </c>
       <c r="D69" s="4" t="s">
         <v>5</v>
       </c>
       <c r="E69" s="4" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F69" s="4">
         <v>498105</v>
       </c>
       <c r="G69" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="H69" s="4"/>
       <c r="I69" s="4" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="J69" s="4" t="s">
+        <v>116</v>
+      </c>
+      <c r="K69" s="4" t="s">
         <v>117</v>
       </c>
-      <c r="K69" s="4" t="s">
-        <v>118</v>
-      </c>
       <c r="L69" s="9" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="M69" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="N69" s="4"/>
     </row>
@@ -4299,486 +4305,486 @@
   <sheetData>
     <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
       <c r="A1" s="12" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="12" t="s">
         <v>135</v>
       </c>
-      <c r="B1" s="12" t="s">
+      <c r="C1" s="12" t="s">
         <v>136</v>
       </c>
-      <c r="C1" s="12" t="s">
+      <c r="D1" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="D1" s="12" t="s">
+      <c r="E1" s="13" t="s">
         <v>138</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="F1" s="12" t="s">
+        <v>125</v>
+      </c>
+      <c r="G1" s="14" t="s">
         <v>139</v>
       </c>
-      <c r="F1" s="12" t="s">
-        <v>126</v>
-      </c>
-      <c r="G1" s="14" t="s">
+      <c r="H1" s="14" t="s">
         <v>140</v>
       </c>
-      <c r="H1" s="14" t="s">
-        <v>141</v>
-      </c>
       <c r="I1" s="12" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A2" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B2" s="15" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="C2" s="15" t="s">
+        <v>141</v>
+      </c>
+      <c r="D2" s="15" t="s">
         <v>142</v>
       </c>
-      <c r="D2" s="15" t="s">
+      <c r="E2" s="15" t="s">
         <v>143</v>
       </c>
-      <c r="E2" s="15" t="s">
+      <c r="F2" s="4" t="s">
         <v>144</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>145</v>
       </c>
       <c r="G2" s="16"/>
       <c r="H2" s="4"/>
       <c r="I2" s="4" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A3" s="4" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B3" s="15" t="s">
+        <v>145</v>
+      </c>
+      <c r="C3" s="15" t="s">
+        <v>96</v>
+      </c>
+      <c r="D3" s="15" t="s">
         <v>146</v>
       </c>
-      <c r="C3" s="15" t="s">
-        <v>97</v>
-      </c>
-      <c r="D3" s="15" t="s">
+      <c r="E3" s="15" t="s">
         <v>147</v>
       </c>
-      <c r="E3" s="15" t="s">
+      <c r="F3" s="4" t="s">
         <v>148</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>149</v>
       </c>
       <c r="G3" s="16"/>
       <c r="H3" s="4"/>
       <c r="I3" s="4" t="s">
-        <v>308</v>
+        <v>307</v>
       </c>
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A4" s="4" t="s">
+        <v>94</v>
+      </c>
+      <c r="B4" s="15" t="s">
         <v>95</v>
-      </c>
-      <c r="B4" s="15" t="s">
-        <v>96</v>
       </c>
       <c r="C4" s="15" t="s">
         <v>7</v>
       </c>
       <c r="D4" s="15" t="s">
+        <v>149</v>
+      </c>
+      <c r="E4" s="15" t="s">
         <v>150</v>
       </c>
-      <c r="E4" s="15" t="s">
+      <c r="F4" s="4" t="s">
         <v>151</v>
-      </c>
-      <c r="F4" s="4" t="s">
-        <v>152</v>
       </c>
       <c r="G4" s="16"/>
       <c r="H4" s="4"/>
       <c r="I4" s="4" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B5" s="15" t="s">
+        <v>152</v>
+      </c>
+      <c r="C5" s="15" t="s">
         <v>153</v>
       </c>
-      <c r="C5" s="15" t="s">
+      <c r="D5" s="15" t="s">
         <v>154</v>
       </c>
-      <c r="D5" s="15" t="s">
+      <c r="E5" s="15" t="s">
         <v>155</v>
       </c>
-      <c r="E5" s="15" t="s">
+      <c r="F5" s="4" t="s">
         <v>156</v>
-      </c>
-      <c r="F5" s="4" t="s">
-        <v>157</v>
       </c>
       <c r="G5" s="16"/>
       <c r="H5" s="4"/>
       <c r="I5" s="4" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B6" s="15" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="C6" s="15" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="D6" s="15" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E6" s="15" t="s">
+        <v>157</v>
+      </c>
+      <c r="F6" s="4" t="s">
         <v>158</v>
-      </c>
-      <c r="F6" s="4" t="s">
-        <v>159</v>
       </c>
       <c r="G6" s="16"/>
       <c r="H6" s="4"/>
       <c r="I6" s="4" t="s">
-        <v>309</v>
+        <v>308</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B7" s="15" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7" s="15" t="s">
         <v>15</v>
       </c>
       <c r="D7" s="15" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E7" s="15" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="F7" s="4" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="G7" s="16"/>
       <c r="H7" s="4"/>
       <c r="I7" s="4" t="s">
-        <v>310</v>
+        <v>309</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B8" s="15" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C8" s="15" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="D8" s="15" t="s">
+        <v>160</v>
+      </c>
+      <c r="E8" s="15" t="s">
         <v>161</v>
-      </c>
-      <c r="E8" s="15" t="s">
-        <v>162</v>
       </c>
       <c r="G8" s="16"/>
       <c r="H8" s="4"/>
       <c r="I8" s="4" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B9" s="15" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="C9" s="15" t="s">
+        <v>162</v>
+      </c>
+      <c r="D9" s="15" t="s">
         <v>163</v>
       </c>
-      <c r="D9" s="15" t="s">
+      <c r="E9" s="15" t="s">
         <v>164</v>
-      </c>
-      <c r="E9" s="15" t="s">
-        <v>165</v>
       </c>
       <c r="G9" s="16"/>
       <c r="H9" s="4"/>
       <c r="I9" s="4" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B10" s="15" t="s">
+        <v>165</v>
+      </c>
+      <c r="C10" s="15" t="s">
         <v>166</v>
       </c>
-      <c r="C10" s="15" t="s">
+      <c r="D10" s="15" t="s">
         <v>167</v>
       </c>
-      <c r="D10" s="15" t="s">
+      <c r="E10" s="17" t="s">
         <v>168</v>
-      </c>
-      <c r="E10" s="17" t="s">
-        <v>169</v>
       </c>
       <c r="G10" s="18">
         <v>0.39069999999999999</v>
       </c>
       <c r="H10" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B11" s="15" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="C11" s="15" t="s">
+        <v>170</v>
+      </c>
+      <c r="D11" s="15" t="s">
         <v>171</v>
       </c>
-      <c r="D11" s="15" t="s">
-        <v>172</v>
-      </c>
       <c r="E11" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G11" s="18">
         <v>0.72446767990114092</v>
       </c>
       <c r="H11" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.35">
       <c r="B12" s="15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C12" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="D12" s="15" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="E12" s="17" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G12" s="18">
         <v>0.59281777811558378</v>
       </c>
       <c r="H12" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I12" s="3"/>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C13" s="15" t="s">
+        <v>173</v>
+      </c>
+      <c r="D13" s="15" t="s">
         <v>174</v>
       </c>
-      <c r="D13" s="15" t="s">
+      <c r="E13" s="17" t="s">
         <v>175</v>
-      </c>
-      <c r="E13" s="17" t="s">
-        <v>176</v>
       </c>
       <c r="G13" s="19">
         <v>1.8120000000000001</v>
       </c>
       <c r="H13" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I13" s="3"/>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C14" s="15" t="s">
+        <v>176</v>
+      </c>
+      <c r="D14" s="15" t="s">
         <v>177</v>
       </c>
-      <c r="D14" s="15" t="s">
-        <v>178</v>
-      </c>
       <c r="E14" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G14" s="19">
         <v>1.8120000000000001</v>
       </c>
       <c r="H14" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I14" s="3"/>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C15" s="15" t="s">
+        <v>178</v>
+      </c>
+      <c r="D15" s="15" t="s">
         <v>179</v>
       </c>
-      <c r="D15" s="15" t="s">
-        <v>180</v>
-      </c>
       <c r="E15" s="17" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G15" s="19">
         <v>1.8120000000000001</v>
       </c>
       <c r="H15" s="21" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="I15" s="3"/>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.35">
       <c r="C16" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="D16" s="15" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="17" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C17" s="15" t="s">
+        <v>181</v>
+      </c>
+      <c r="D17" s="15" t="s">
         <v>182</v>
-      </c>
-      <c r="D17" s="15" t="s">
-        <v>183</v>
       </c>
     </row>
     <row r="18" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C18" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="D18" s="15" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="19" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C19" s="15" t="s">
+        <v>184</v>
+      </c>
+      <c r="D19" s="15" t="s">
         <v>185</v>
-      </c>
-      <c r="D19" s="15" t="s">
-        <v>186</v>
       </c>
     </row>
     <row r="20" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C20" s="15" t="s">
+        <v>186</v>
+      </c>
+      <c r="D20" s="15" t="s">
         <v>187</v>
-      </c>
-      <c r="D20" s="15" t="s">
-        <v>188</v>
       </c>
     </row>
     <row r="21" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C21" s="15" t="s">
+        <v>188</v>
+      </c>
+      <c r="D21" s="15" t="s">
         <v>189</v>
-      </c>
-      <c r="D21" s="15" t="s">
-        <v>190</v>
       </c>
     </row>
     <row r="22" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C22" s="15" t="s">
+        <v>190</v>
+      </c>
+      <c r="D22" s="15" t="s">
         <v>191</v>
-      </c>
-      <c r="D22" s="15" t="s">
-        <v>192</v>
       </c>
     </row>
     <row r="23" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C23" s="15" t="s">
+        <v>192</v>
+      </c>
+      <c r="D23" s="15" t="s">
         <v>193</v>
-      </c>
-      <c r="D23" s="15" t="s">
-        <v>194</v>
       </c>
     </row>
     <row r="24" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C24" s="15" t="s">
+        <v>194</v>
+      </c>
+      <c r="D24" s="15" t="s">
         <v>195</v>
-      </c>
-      <c r="D24" s="15" t="s">
-        <v>196</v>
       </c>
     </row>
     <row r="25" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C25" s="15" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="15" t="s">
         <v>197</v>
-      </c>
-      <c r="D25" s="15" t="s">
-        <v>198</v>
       </c>
     </row>
     <row r="26" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C26" s="15" t="s">
+        <v>198</v>
+      </c>
+      <c r="D26" s="15" t="s">
         <v>199</v>
-      </c>
-      <c r="D26" s="15" t="s">
-        <v>200</v>
       </c>
     </row>
     <row r="27" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C27" s="15" t="s">
+        <v>200</v>
+      </c>
+      <c r="D27" s="15" t="s">
         <v>201</v>
-      </c>
-      <c r="D27" s="15" t="s">
-        <v>202</v>
       </c>
     </row>
     <row r="28" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C28" s="15" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="D28" s="15" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
     </row>
     <row r="29" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C29" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="D29" s="15" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
     </row>
     <row r="30" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C30" s="15" t="s">
+        <v>204</v>
+      </c>
+      <c r="D30" s="15" t="s">
         <v>205</v>
-      </c>
-      <c r="D30" s="15" t="s">
-        <v>206</v>
       </c>
     </row>
     <row r="31" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C31" s="15" t="s">
+        <v>206</v>
+      </c>
+      <c r="D31" s="15" t="s">
         <v>207</v>
-      </c>
-      <c r="D31" s="15" t="s">
-        <v>208</v>
       </c>
     </row>
     <row r="32" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C32" s="15" t="s">
+        <v>208</v>
+      </c>
+      <c r="D32" s="15" t="s">
         <v>209</v>
-      </c>
-      <c r="D32" s="15" t="s">
-        <v>210</v>
       </c>
     </row>
     <row r="33" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C33" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="D33" s="15" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="34" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C34" s="15" t="s">
+        <v>211</v>
+      </c>
+      <c r="D34" s="15" t="s">
         <v>212</v>
-      </c>
-      <c r="D34" s="15" t="s">
-        <v>213</v>
       </c>
     </row>
     <row r="35" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C35" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="D35" s="15" t="s">
         <v>0</v>
@@ -4786,266 +4792,266 @@
     </row>
     <row r="36" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C36" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="D36" s="15" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="37" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C37" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="D37" s="15" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="38" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C38" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="D38" s="15" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
     </row>
     <row r="39" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C39" s="15" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="D39" s="15" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="40" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C40" s="15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="D40" s="15" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="41" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C41" s="15" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="D41" s="15" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="42" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C42" s="15" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="D42" s="15" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="43" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C43" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="D43" s="15" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="44" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C44" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="D44" s="15" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="45" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C45" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="D45" s="15" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="46" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C46" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="D46" s="15" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="47" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C47" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="D47" s="15" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="48" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C48" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="D48" s="15" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="49" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C49" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="D49" s="15" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="50" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C50" s="15" t="s">
+        <v>222</v>
+      </c>
+      <c r="D50" s="15" t="s">
         <v>223</v>
-      </c>
-      <c r="D50" s="15" t="s">
-        <v>224</v>
       </c>
     </row>
     <row r="51" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C51" s="15" t="s">
+        <v>224</v>
+      </c>
+      <c r="D51" s="15" t="s">
         <v>225</v>
-      </c>
-      <c r="D51" s="15" t="s">
-        <v>226</v>
       </c>
     </row>
     <row r="52" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C52" s="15" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="D52" s="15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="53" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C53" s="15" t="s">
+        <v>226</v>
+      </c>
+      <c r="D53" s="15" t="s">
         <v>227</v>
-      </c>
-      <c r="D53" s="15" t="s">
-        <v>228</v>
       </c>
     </row>
     <row r="54" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C54" s="15" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="D54" s="15" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
     </row>
     <row r="55" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C55" s="15" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="D55" s="15" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="56" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C56" s="15" t="s">
+        <v>230</v>
+      </c>
+      <c r="D56" s="15" t="s">
         <v>231</v>
-      </c>
-      <c r="D56" s="15" t="s">
-        <v>232</v>
       </c>
     </row>
     <row r="57" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C57" s="15" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="D57" s="15" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
     </row>
     <row r="58" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C58" s="15" t="s">
+        <v>233</v>
+      </c>
+      <c r="D58" s="15" t="s">
         <v>234</v>
-      </c>
-      <c r="D58" s="15" t="s">
-        <v>235</v>
       </c>
     </row>
     <row r="59" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C59" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="D59" s="15" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="60" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C60" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="D60" s="15" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="61" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C61" s="15" t="s">
+        <v>237</v>
+      </c>
+      <c r="D61" s="15" t="s">
         <v>238</v>
-      </c>
-      <c r="D61" s="15" t="s">
-        <v>239</v>
       </c>
     </row>
     <row r="62" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C62" s="15" t="s">
+        <v>239</v>
+      </c>
+      <c r="D62" s="15" t="s">
         <v>240</v>
-      </c>
-      <c r="D62" s="15" t="s">
-        <v>241</v>
       </c>
     </row>
     <row r="63" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C63" s="15" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="D63" s="15" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
     </row>
     <row r="64" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C64" s="15" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="D64" s="15" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="65" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C65" s="15" t="s">
+        <v>243</v>
+      </c>
+      <c r="D65" s="15" t="s">
         <v>244</v>
-      </c>
-      <c r="D65" s="15" t="s">
-        <v>245</v>
       </c>
     </row>
     <row r="66" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C66" s="15" t="s">
+        <v>245</v>
+      </c>
+      <c r="D66" s="15" t="s">
         <v>246</v>
-      </c>
-      <c r="D66" s="15" t="s">
-        <v>247</v>
       </c>
     </row>
     <row r="67" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C67" s="15" t="s">
+        <v>247</v>
+      </c>
+      <c r="D67" s="15" t="s">
         <v>248</v>
-      </c>
-      <c r="D67" s="15" t="s">
-        <v>249</v>
       </c>
     </row>
     <row r="68" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C68" s="15" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="D68" s="15" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
     </row>
     <row r="69" spans="3:4" x14ac:dyDescent="0.35">
@@ -5053,466 +5059,466 @@
         <v>33</v>
       </c>
       <c r="D69" s="15" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
     </row>
     <row r="70" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C70" s="20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="D70" s="15" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
     </row>
     <row r="71" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C71" s="20" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="D71" s="15" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="72" spans="3:4" x14ac:dyDescent="0.35">
       <c r="C72" s="20" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="D72" s="15" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
     </row>
     <row r="73" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D73" s="15" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
     </row>
     <row r="74" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D74" s="15" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
     </row>
     <row r="75" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D75" s="15" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
     </row>
     <row r="76" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D76" s="15" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
     </row>
     <row r="77" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D77" s="15" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
     </row>
     <row r="78" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D78" s="15" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="79" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D79" s="15" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="80" spans="3:4" x14ac:dyDescent="0.35">
       <c r="D80" s="15" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
     </row>
     <row r="81" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D81" s="15" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="82" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D82" s="15" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
     </row>
     <row r="83" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D83" s="15" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
     </row>
     <row r="84" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D84" s="15" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
     </row>
     <row r="85" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D85" s="15" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
     </row>
     <row r="86" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D86" s="15" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
     </row>
     <row r="87" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D87" s="15" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
     </row>
     <row r="88" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D88" s="15" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
     </row>
     <row r="89" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D89" s="15" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
     </row>
     <row r="90" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D90" s="15" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
     </row>
     <row r="91" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D91" s="15" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
     </row>
     <row r="92" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D92" s="15" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
     </row>
     <row r="93" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D93" s="15" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
     </row>
     <row r="94" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D94" s="15" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="95" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D95" s="15" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="96" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D96" s="15" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="97" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D97" s="15" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
     </row>
     <row r="98" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D98" s="15" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
     </row>
     <row r="99" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D99" s="15" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
     </row>
     <row r="100" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D100" s="15" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
     </row>
     <row r="101" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D101" s="15" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
     </row>
     <row r="102" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D102" s="15" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
     </row>
     <row r="103" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D103" s="15" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
     </row>
     <row r="104" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D104" s="15" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
     </row>
     <row r="105" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D105" s="15" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D106" s="15" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
     </row>
     <row r="107" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D107" s="15" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
     </row>
     <row r="108" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D108" s="15" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
     </row>
     <row r="109" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D109" s="15" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
     </row>
     <row r="110" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D110" s="15" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
     </row>
     <row r="111" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D111" s="15" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
     </row>
     <row r="112" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D112" s="15" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
     </row>
     <row r="113" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D113" s="15" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
     </row>
     <row r="114" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D114" s="15" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
     </row>
     <row r="115" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D115" s="15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="116" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D116" s="15" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="117" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D117" s="15" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="118" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D118" s="15" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="119" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D119" s="15" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
     </row>
     <row r="120" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D120" s="15" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
     </row>
     <row r="121" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D121" s="15" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
     </row>
     <row r="122" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D122" s="15" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="123" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D123" s="15" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
     </row>
     <row r="124" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D124" s="15" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
     </row>
     <row r="125" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D125" s="15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="126" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D126" s="15" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
     </row>
     <row r="127" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D127" s="15" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="128" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D128" s="15" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="129" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D129" s="15" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
     </row>
     <row r="130" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D130" s="15" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
     </row>
     <row r="131" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D131" s="15" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
     </row>
     <row r="132" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D132" s="15" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
     </row>
     <row r="133" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D133" s="15" t="s">
-        <v>287</v>
+        <v>286</v>
       </c>
     </row>
     <row r="134" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D134" s="15" t="s">
-        <v>288</v>
+        <v>287</v>
       </c>
     </row>
     <row r="135" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D135" s="15" t="s">
-        <v>289</v>
+        <v>288</v>
       </c>
     </row>
     <row r="136" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D136" s="15" t="s">
-        <v>290</v>
+        <v>289</v>
       </c>
     </row>
     <row r="137" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D137" s="15" t="s">
-        <v>291</v>
+        <v>290</v>
       </c>
     </row>
     <row r="138" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D138" s="15" t="s">
-        <v>292</v>
+        <v>291</v>
       </c>
     </row>
     <row r="139" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D139" s="15" t="s">
-        <v>293</v>
+        <v>292</v>
       </c>
     </row>
     <row r="140" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D140" s="15" t="s">
-        <v>294</v>
+        <v>293</v>
       </c>
     </row>
     <row r="141" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D141" s="15" t="s">
-        <v>295</v>
+        <v>294</v>
       </c>
     </row>
     <row r="142" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D142" s="15" t="s">
-        <v>296</v>
+        <v>295</v>
       </c>
     </row>
     <row r="143" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D143" s="15" t="s">
-        <v>297</v>
+        <v>296</v>
       </c>
     </row>
     <row r="144" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D144" s="15" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
     </row>
     <row r="145" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D145" s="15" t="s">
-        <v>299</v>
+        <v>298</v>
       </c>
     </row>
     <row r="146" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D146" s="15" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="147" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D147" s="15" t="s">
-        <v>300</v>
+        <v>299</v>
       </c>
     </row>
     <row r="148" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D148" s="15" t="s">
-        <v>301</v>
+        <v>300</v>
       </c>
     </row>
     <row r="149" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D149" s="15" t="s">
-        <v>302</v>
+        <v>301</v>
       </c>
     </row>
     <row r="150" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D150" s="15" t="s">
-        <v>303</v>
+        <v>302</v>
       </c>
     </row>
     <row r="151" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D151" s="15" t="s">
-        <v>304</v>
+        <v>303</v>
       </c>
     </row>
     <row r="152" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D152" s="15" t="s">
-        <v>305</v>
+        <v>304</v>
       </c>
     </row>
     <row r="153" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D153" s="20" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="154" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D154" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="155" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D155" s="20" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="156" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D156" s="20" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="157" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D157" s="20" t="s">
-        <v>306</v>
+        <v>305</v>
       </c>
     </row>
     <row r="158" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D158" s="20" t="s">
-        <v>307</v>
+        <v>306</v>
       </c>
     </row>
     <row r="159" spans="4:4" x14ac:dyDescent="0.35">
       <c r="D159" s="20" t="s">
-        <v>311</v>
+        <v>310</v>
       </c>
     </row>
   </sheetData>

</xml_diff>